<commit_message>
Highlight data used in Population_validation_targets Excel doc.
</commit_message>
<xml_diff>
--- a/Config/Population_validation_targets.xlsx
+++ b/Config/Population_validation_targets.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -391,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -480,8 +479,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5201,8 +5202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V73" sqref="V73"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5301,10 +5302,10 @@
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="45">
         <v>1950</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="46">
         <v>6.05</v>
       </c>
       <c r="D4" s="4"/>
@@ -5319,11 +5320,11 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="45">
         <f>B4+5</f>
         <v>1955</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="46">
         <v>6.05</v>
       </c>
       <c r="D5" s="4"/>
@@ -5335,11 +5336,11 @@
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="45">
         <f t="shared" ref="B6:B33" si="0">B5+5</f>
         <v>1960</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="46">
         <v>6</v>
       </c>
       <c r="D6" s="4"/>
@@ -5351,11 +5352,11 @@
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="45">
         <f t="shared" si="0"/>
         <v>1965</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="46">
         <v>5.8</v>
       </c>
       <c r="D7" s="4"/>
@@ -5367,11 +5368,11 @@
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="45">
         <f t="shared" si="0"/>
         <v>1970</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="46">
         <v>5.5</v>
       </c>
       <c r="D8" s="4"/>
@@ -5383,11 +5384,11 @@
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="45">
         <f t="shared" si="0"/>
         <v>1975</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="46">
         <v>5.05</v>
       </c>
       <c r="D9" s="4"/>
@@ -5399,11 +5400,11 @@
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="45">
         <f t="shared" si="0"/>
         <v>1980</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="46">
         <v>4.899</v>
       </c>
       <c r="D10" s="4"/>
@@ -5415,11 +5416,11 @@
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="45">
         <f t="shared" si="0"/>
         <v>1985</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="46">
         <v>4.4000000000000004</v>
       </c>
       <c r="D11" s="4"/>
@@ -5431,11 +5432,11 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="45">
         <f t="shared" si="0"/>
         <v>1990</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="46">
         <v>3.5070000000000001</v>
       </c>
       <c r="D12" s="4"/>
@@ -5447,11 +5448,11 @@
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="45">
         <f t="shared" si="0"/>
         <v>1995</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="46">
         <v>2.8763000000000001</v>
       </c>
       <c r="D13" s="4"/>
@@ -5463,11 +5464,11 @@
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="45">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="46">
         <v>2.6124999999999998</v>
       </c>
       <c r="D14" s="4"/>
@@ -5479,11 +5480,11 @@
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="45">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="46">
         <v>2.625</v>
       </c>
       <c r="D15" s="4"/>
@@ -5495,11 +5496,11 @@
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="45">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="46">
         <v>2.5499999999999998</v>
       </c>
       <c r="D16" s="4"/>
@@ -5511,11 +5512,11 @@
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="45">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="46">
         <v>2.4138999999999999</v>
       </c>
       <c r="D17" s="4"/>
@@ -5527,11 +5528,11 @@
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="45">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="46">
         <v>2.3088000000000002</v>
       </c>
       <c r="D18" s="5">
@@ -5569,11 +5570,11 @@
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="45">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="46">
         <v>2.2183000000000002</v>
       </c>
       <c r="D19" s="5">
@@ -5593,11 +5594,11 @@
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="45">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="46">
         <v>2.1366000000000001</v>
       </c>
       <c r="D20" s="5">
@@ -5617,11 +5618,11 @@
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="45">
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="46">
         <v>2.0691999999999999</v>
       </c>
       <c r="D21" s="5">
@@ -5641,11 +5642,11 @@
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="45">
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="46">
         <v>2.0045000000000002</v>
       </c>
       <c r="D22" s="5">
@@ -5665,11 +5666,11 @@
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="45">
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="46">
         <v>1.9553</v>
       </c>
       <c r="D23" s="5">
@@ -5689,11 +5690,11 @@
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="45">
         <f t="shared" si="0"/>
         <v>2050</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="46">
         <v>1.9147000000000001</v>
       </c>
       <c r="D24" s="5">
@@ -5713,11 +5714,11 @@
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="45">
         <f t="shared" si="0"/>
         <v>2055</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="46">
         <v>1.8793</v>
       </c>
       <c r="D25" s="5">
@@ -5737,11 +5738,11 @@
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="45">
         <f t="shared" si="0"/>
         <v>2060</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="46">
         <v>1.8522000000000001</v>
       </c>
       <c r="D26" s="5">
@@ -5761,11 +5762,11 @@
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="45">
         <f t="shared" si="0"/>
         <v>2065</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="46">
         <v>1.8292999999999999</v>
       </c>
       <c r="D27" s="5">
@@ -5785,11 +5786,11 @@
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="45">
         <f t="shared" si="0"/>
         <v>2070</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="46">
         <v>1.8130999999999999</v>
       </c>
       <c r="D28" s="5">
@@ -5809,11 +5810,11 @@
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="45">
         <f t="shared" si="0"/>
         <v>2075</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="46">
         <v>1.8006</v>
       </c>
       <c r="D29" s="5">
@@ -5833,11 +5834,11 @@
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="45">
         <f t="shared" si="0"/>
         <v>2080</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="46">
         <v>1.7890999999999999</v>
       </c>
       <c r="D30" s="5">
@@ -5857,11 +5858,11 @@
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="45">
         <f t="shared" si="0"/>
         <v>2085</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="46">
         <v>1.7819</v>
       </c>
       <c r="D31" s="5">
@@ -5881,11 +5882,11 @@
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="45">
         <f t="shared" si="0"/>
         <v>2090</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="46">
         <v>1.7778</v>
       </c>
       <c r="D32" s="5">
@@ -5905,11 +5906,11 @@
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="45">
         <f t="shared" si="0"/>
         <v>2095</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="46">
         <v>1.7734000000000001</v>
       </c>
       <c r="D33" s="4">
@@ -8326,19 +8327,19 @@
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A91" s="7"/>
-      <c r="B91" s="7">
+      <c r="B91" s="45">
         <v>1996</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="45">
         <v>2001</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D91" s="45">
         <v>2011</v>
       </c>
-      <c r="E91" s="7">
+      <c r="E91" s="45">
         <v>2016</v>
       </c>
-      <c r="F91" s="7">
+      <c r="F91" s="45">
         <v>2019</v>
       </c>
       <c r="G91" s="28"/>
@@ -8934,8 +8935,12 @@
       <c r="C111" s="7">
         <v>2001</v>
       </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="4"/>
+      <c r="D111" s="7">
+        <v>2011</v>
+      </c>
+      <c r="E111" s="7">
+        <v>2016</v>
+      </c>
       <c r="F111" s="7">
         <v>2019</v>
       </c>
@@ -9429,23 +9434,23 @@
       <c r="A130" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="1">
         <f>B129/1000</f>
         <v>8080.1360000000004</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="1">
         <f t="shared" ref="C130:F130" si="7">C129/1000</f>
         <v>9143.8979999999992</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="1">
         <f t="shared" si="7"/>
         <v>9934.9220000000005</v>
       </c>
-      <c r="E130">
+      <c r="E130" s="1">
         <f t="shared" si="7"/>
         <v>10757.89</v>
       </c>
-      <c r="F130">
+      <c r="F130" s="1">
         <f t="shared" si="7"/>
         <v>10907.773999999999</v>
       </c>
@@ -9727,120 +9732,120 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" s="4"/>
-      <c r="B144" s="7">
+      <c r="B144" s="45">
         <v>2025</v>
       </c>
-      <c r="C144" s="7">
+      <c r="C144" s="45">
         <v>2030</v>
       </c>
-      <c r="D144" s="7">
+      <c r="D144" s="45">
         <v>2035</v>
       </c>
-      <c r="E144" s="7">
+      <c r="E144" s="45">
         <v>2040</v>
       </c>
-      <c r="F144" s="7">
+      <c r="F144" s="45">
         <v>2045</v>
       </c>
-      <c r="G144" s="7">
+      <c r="G144" s="45">
         <v>2050</v>
       </c>
-      <c r="H144" s="7">
+      <c r="H144" s="45">
         <v>2055</v>
       </c>
-      <c r="I144" s="7">
+      <c r="I144" s="45">
         <v>2060</v>
       </c>
-      <c r="J144" s="7">
+      <c r="J144" s="45">
         <v>2065</v>
       </c>
-      <c r="K144" s="7">
+      <c r="K144" s="45">
         <v>2070</v>
       </c>
-      <c r="L144" s="7">
+      <c r="L144" s="45">
         <v>2075</v>
       </c>
-      <c r="M144" s="7">
+      <c r="M144" s="45">
         <v>2080</v>
       </c>
-      <c r="N144" s="7">
+      <c r="N144" s="45">
         <v>2085</v>
       </c>
-      <c r="O144" s="7">
+      <c r="O144" s="45">
         <v>2090</v>
       </c>
-      <c r="P144" s="7">
+      <c r="P144" s="45">
         <v>2095</v>
       </c>
-      <c r="Q144" s="7">
+      <c r="Q144" s="45">
         <v>2100</v>
       </c>
     </row>
     <row r="145" spans="1:17" ht="116" x14ac:dyDescent="0.35">
-      <c r="A145" s="44" t="s">
+      <c r="A145" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B145" s="4">
+      <c r="B145" s="44">
         <f>(($B142*B144+$A142)/100)*B83</f>
         <v>11232.769782500007</v>
       </c>
-      <c r="C145" s="4">
+      <c r="C145" s="44">
         <f t="shared" ref="C145:Q145" si="9">(($B142*C144+$A142)/100)*C83</f>
         <v>11438.18222328</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D145" s="44">
         <f t="shared" si="9"/>
         <v>11561.455342979998</v>
       </c>
-      <c r="E145" s="4">
+      <c r="E145" s="44">
         <f t="shared" si="9"/>
         <v>11601.144488280008</v>
       </c>
-      <c r="F145" s="4">
+      <c r="F145" s="44">
         <f t="shared" si="9"/>
         <v>11555.878831380005</v>
       </c>
-      <c r="G145" s="4">
+      <c r="G145" s="44">
         <f t="shared" si="9"/>
         <v>11423.608762499996</v>
       </c>
-      <c r="H145" s="4">
+      <c r="H145" s="44">
         <f t="shared" si="9"/>
         <v>11172.059938899991</v>
       </c>
-      <c r="I145" s="4">
+      <c r="I145" s="44">
         <f t="shared" si="9"/>
         <v>10849.798171380005</v>
       </c>
-      <c r="J145" s="4">
+      <c r="J145" s="44">
         <f t="shared" si="9"/>
         <v>10527.866247959999</v>
       </c>
-      <c r="K145" s="4">
+      <c r="K145" s="44">
         <f t="shared" si="9"/>
         <v>10211.048344719989</v>
       </c>
-      <c r="L145" s="4">
+      <c r="L145" s="44">
         <f t="shared" si="9"/>
         <v>9871.7309883000053</v>
       </c>
-      <c r="M145" s="4">
+      <c r="M145" s="44">
         <f t="shared" si="9"/>
         <v>9465.8934329200001</v>
       </c>
-      <c r="N145" s="4">
+      <c r="N145" s="44">
         <f t="shared" si="9"/>
         <v>9025.2317390799908</v>
       </c>
-      <c r="O145" s="4">
+      <c r="O145" s="44">
         <f t="shared" si="9"/>
         <v>8586.6460133400069</v>
       </c>
-      <c r="P145" s="4">
+      <c r="P145" s="44">
         <f t="shared" si="9"/>
         <v>8154.376048420002</v>
       </c>
-      <c r="Q145" s="4">
+      <c r="Q145" s="44">
         <f t="shared" si="9"/>
         <v>7726.0072344999935</v>
       </c>
@@ -9862,16 +9867,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modify KZN validation population predictions to assume KZN remains the same proportion of the total SA population after 2019.
</commit_message>
<xml_diff>
--- a/Config/Population_validation_targets.xlsx
+++ b/Config/Population_validation_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
   <si>
     <t>1950-1955</t>
   </si>
@@ -259,6 +259,12 @@
   <si>
     <t>Projected total number calculated as propotion of UN South Africa estimates</t>
   </si>
+  <si>
+    <t>continued decrease in proportion</t>
+  </si>
+  <si>
+    <t>proportion stabilizes after 2019</t>
+  </si>
 </sst>
 </file>
 
@@ -390,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -411,9 +417,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,27 +429,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -461,12 +443,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,6 +459,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2339,7 +2349,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Projected KZN as proportion of SSA est.</c:v>
+            <c:v>Projected KZN as proportion of SSA est. (assume stabilized proportion after 2019)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2365,7 +2375,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$144:$Q$144</c:f>
+              <c:f>Demographics!$C$144:$R$144</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -2422,57 +2432,57 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$145:$Q$145</c:f>
+              <c:f>Demographics!$C$146:$R$146</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>11232.769782500007</c:v>
+                  <c:v>11626.37088</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11438.18222328</c:v>
+                  <c:v>12156.155135999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11561.455342979998</c:v>
+                  <c:v>12625.409088000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11601.144488280008</c:v>
+                  <c:v>13027.370112000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11555.878831380005</c:v>
+                  <c:v>13354.572864000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11423.608762499996</c:v>
+                  <c:v>13597.848</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11172.059938899991</c:v>
+                  <c:v>13709.80128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10849.798171380005</c:v>
+                  <c:v>13739.356608000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10527.866247959999</c:v>
+                  <c:v>13771.292544000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10211.048344719989</c:v>
+                  <c:v>13812.324095999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9871.7309883000053</c:v>
+                  <c:v>13824.743615999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9465.8934329200001</c:v>
+                  <c:v>13741.505664</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9025.2317390799908</c:v>
+                  <c:v>13599.470207999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8586.6460133400069</c:v>
+                  <c:v>13449.470016000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8154.376048420002</c:v>
+                  <c:v>13297.436736000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7726.0072344999935</c:v>
+                  <c:v>13139.002559999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5200,10 +5210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA145"/>
+  <dimension ref="A1:AA146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I152" sqref="I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5218,16 +5228,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -5249,16 +5259,16 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5302,10 +5312,10 @@
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="35">
         <v>1950</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="36">
         <v>6.05</v>
       </c>
       <c r="D4" s="4"/>
@@ -5320,11 +5330,11 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="35">
         <f>B4+5</f>
         <v>1955</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="36">
         <v>6.05</v>
       </c>
       <c r="D5" s="4"/>
@@ -5336,11 +5346,11 @@
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="35">
         <f t="shared" ref="B6:B33" si="0">B5+5</f>
         <v>1960</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="36">
         <v>6</v>
       </c>
       <c r="D6" s="4"/>
@@ -5352,11 +5362,11 @@
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="35">
         <f t="shared" si="0"/>
         <v>1965</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="36">
         <v>5.8</v>
       </c>
       <c r="D7" s="4"/>
@@ -5368,11 +5378,11 @@
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="35">
         <f t="shared" si="0"/>
         <v>1970</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="36">
         <v>5.5</v>
       </c>
       <c r="D8" s="4"/>
@@ -5384,11 +5394,11 @@
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="35">
         <f t="shared" si="0"/>
         <v>1975</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="36">
         <v>5.05</v>
       </c>
       <c r="D9" s="4"/>
@@ -5400,11 +5410,11 @@
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="35">
         <f t="shared" si="0"/>
         <v>1980</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="36">
         <v>4.899</v>
       </c>
       <c r="D10" s="4"/>
@@ -5416,11 +5426,11 @@
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="35">
         <f t="shared" si="0"/>
         <v>1985</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="36">
         <v>4.4000000000000004</v>
       </c>
       <c r="D11" s="4"/>
@@ -5432,11 +5442,11 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="35">
         <f t="shared" si="0"/>
         <v>1990</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="36">
         <v>3.5070000000000001</v>
       </c>
       <c r="D12" s="4"/>
@@ -5448,11 +5458,11 @@
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B13" s="35">
         <f t="shared" si="0"/>
         <v>1995</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="36">
         <v>2.8763000000000001</v>
       </c>
       <c r="D13" s="4"/>
@@ -5464,11 +5474,11 @@
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="35">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="36">
         <v>2.6124999999999998</v>
       </c>
       <c r="D14" s="4"/>
@@ -5480,11 +5490,11 @@
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B15" s="35">
         <f t="shared" si="0"/>
         <v>2005</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="36">
         <v>2.625</v>
       </c>
       <c r="D15" s="4"/>
@@ -5496,11 +5506,11 @@
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B16" s="35">
         <f t="shared" si="0"/>
         <v>2010</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="36">
         <v>2.5499999999999998</v>
       </c>
       <c r="D16" s="4"/>
@@ -5512,11 +5522,11 @@
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="45">
+      <c r="B17" s="35">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="36">
         <v>2.4138999999999999</v>
       </c>
       <c r="D17" s="4"/>
@@ -5528,11 +5538,11 @@
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B18" s="35">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="36">
         <v>2.3088000000000002</v>
       </c>
       <c r="D18" s="5">
@@ -5570,11 +5580,11 @@
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="45">
+      <c r="B19" s="35">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="36">
         <v>2.2183000000000002</v>
       </c>
       <c r="D19" s="5">
@@ -5594,11 +5604,11 @@
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B20" s="35">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20" s="36">
         <v>2.1366000000000001</v>
       </c>
       <c r="D20" s="5">
@@ -5618,11 +5628,11 @@
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="45">
+      <c r="B21" s="35">
         <f t="shared" si="0"/>
         <v>2035</v>
       </c>
-      <c r="C21" s="46">
+      <c r="C21" s="36">
         <v>2.0691999999999999</v>
       </c>
       <c r="D21" s="5">
@@ -5642,11 +5652,11 @@
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B22" s="35">
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22" s="36">
         <v>2.0045000000000002</v>
       </c>
       <c r="D22" s="5">
@@ -5666,11 +5676,11 @@
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B23" s="35">
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
-      <c r="C23" s="46">
+      <c r="C23" s="36">
         <v>1.9553</v>
       </c>
       <c r="D23" s="5">
@@ -5690,11 +5700,11 @@
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B24" s="35">
         <f t="shared" si="0"/>
         <v>2050</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C24" s="36">
         <v>1.9147000000000001</v>
       </c>
       <c r="D24" s="5">
@@ -5714,11 +5724,11 @@
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="45">
+      <c r="B25" s="35">
         <f t="shared" si="0"/>
         <v>2055</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C25" s="36">
         <v>1.8793</v>
       </c>
       <c r="D25" s="5">
@@ -5738,11 +5748,11 @@
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="35">
         <f t="shared" si="0"/>
         <v>2060</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="36">
         <v>1.8522000000000001</v>
       </c>
       <c r="D26" s="5">
@@ -5762,11 +5772,11 @@
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="45">
+      <c r="B27" s="35">
         <f t="shared" si="0"/>
         <v>2065</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="36">
         <v>1.8292999999999999</v>
       </c>
       <c r="D27" s="5">
@@ -5786,11 +5796,11 @@
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="35">
         <f t="shared" si="0"/>
         <v>2070</v>
       </c>
-      <c r="C28" s="46">
+      <c r="C28" s="36">
         <v>1.8130999999999999</v>
       </c>
       <c r="D28" s="5">
@@ -5810,11 +5820,11 @@
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="45">
+      <c r="B29" s="35">
         <f t="shared" si="0"/>
         <v>2075</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="36">
         <v>1.8006</v>
       </c>
       <c r="D29" s="5">
@@ -5834,11 +5844,11 @@
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="45">
+      <c r="B30" s="35">
         <f t="shared" si="0"/>
         <v>2080</v>
       </c>
-      <c r="C30" s="46">
+      <c r="C30" s="36">
         <v>1.7890999999999999</v>
       </c>
       <c r="D30" s="5">
@@ -5858,11 +5868,11 @@
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="45">
+      <c r="B31" s="35">
         <f t="shared" si="0"/>
         <v>2085</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C31" s="36">
         <v>1.7819</v>
       </c>
       <c r="D31" s="5">
@@ -5882,11 +5892,11 @@
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="45">
+      <c r="B32" s="35">
         <f t="shared" si="0"/>
         <v>2090</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="36">
         <v>1.7778</v>
       </c>
       <c r="D32" s="5">
@@ -5906,11 +5916,11 @@
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="45">
+      <c r="B33" s="35">
         <f t="shared" si="0"/>
         <v>2095</v>
       </c>
-      <c r="C33" s="46">
+      <c r="C33" s="36">
         <v>1.7734000000000001</v>
       </c>
       <c r="D33" s="4">
@@ -5927,16 +5937,16 @@
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -5958,16 +5968,16 @@
       <c r="AA36" s="1"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -5988,25 +5998,25 @@
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" spans="1:27" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="24" t="s">
+    <row r="38" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
-      <c r="P38" s="26"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="46"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
@@ -6057,7 +6067,7 @@
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="4">
@@ -6107,7 +6117,7 @@
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="4">
@@ -6157,7 +6167,7 @@
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="4">
@@ -6207,7 +6217,7 @@
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="4">
@@ -6257,7 +6267,7 @@
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="4">
@@ -6307,7 +6317,7 @@
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="4">
@@ -6357,7 +6367,7 @@
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="4">
@@ -6407,7 +6417,7 @@
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="4">
@@ -6457,7 +6467,7 @@
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="4">
@@ -6507,7 +6517,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="4">
@@ -6557,7 +6567,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="4">
@@ -6607,7 +6617,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="4">
@@ -6657,7 +6667,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="4">
@@ -6707,7 +6717,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="4">
@@ -6757,7 +6767,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="4">
@@ -6807,7 +6817,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B55" s="4">
@@ -6857,7 +6867,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B56">
@@ -6922,27 +6932,27 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A57" s="11"/>
+      <c r="A57" s="10"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
-      <c r="N58" s="21"/>
-      <c r="O58" s="21"/>
-      <c r="P58" s="22"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="40"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="40"/>
+      <c r="N58" s="40"/>
+      <c r="O58" s="40"/>
+      <c r="P58" s="41"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="7"/>
@@ -6993,7 +7003,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B60" s="4">
@@ -7043,7 +7053,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B61" s="4">
@@ -7093,7 +7103,7 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B62" s="4">
@@ -7143,7 +7153,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B63" s="4">
@@ -7193,7 +7203,7 @@
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="4">
@@ -7243,7 +7253,7 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B65" s="4">
@@ -7293,7 +7303,7 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B66" s="4">
@@ -7343,7 +7353,7 @@
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B67" s="4">
@@ -7393,7 +7403,7 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B68" s="4">
@@ -7443,7 +7453,7 @@
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B69" s="4">
@@ -7493,7 +7503,7 @@
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B70" s="4">
@@ -7543,7 +7553,7 @@
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B71" s="4">
@@ -7593,7 +7603,7 @@
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B72" s="4">
@@ -7643,7 +7653,7 @@
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B73" s="4">
@@ -7693,7 +7703,7 @@
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B74" s="4">
@@ -7743,7 +7753,7 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B75" s="4">
@@ -7793,7 +7803,7 @@
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A76" s="18" t="s">
+      <c r="A76" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B76">
@@ -7858,7 +7868,7 @@
       </c>
     </row>
     <row r="77" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B77">
@@ -7923,25 +7933,25 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="23"/>
-      <c r="H79" s="23"/>
-      <c r="I79" s="23"/>
-      <c r="J79" s="23"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="23"/>
-      <c r="M79" s="23"/>
-      <c r="N79" s="23"/>
-      <c r="O79" s="23"/>
-      <c r="P79" s="23"/>
-      <c r="Q79" s="23"/>
+      <c r="B79" s="42"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="42"/>
+      <c r="H79" s="42"/>
+      <c r="I79" s="42"/>
+      <c r="J79" s="42"/>
+      <c r="K79" s="42"/>
+      <c r="L79" s="42"/>
+      <c r="M79" s="42"/>
+      <c r="N79" s="42"/>
+      <c r="O79" s="42"/>
+      <c r="P79" s="42"/>
+      <c r="Q79" s="42"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="4"/>
@@ -7998,190 +8008,190 @@
       <c r="A81" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="15">
+      <c r="B81" s="14">
         <v>27699</v>
       </c>
-      <c r="C81" s="15">
+      <c r="C81" s="14">
         <v>28352</v>
       </c>
-      <c r="D81" s="15">
+      <c r="D81" s="14">
         <v>28398</v>
       </c>
-      <c r="E81" s="15">
+      <c r="E81" s="14">
         <v>28126</v>
       </c>
-      <c r="F81" s="15">
+      <c r="F81" s="14">
         <v>27873</v>
       </c>
-      <c r="G81" s="15">
+      <c r="G81" s="14">
         <v>27634</v>
       </c>
-      <c r="H81" s="15">
+      <c r="H81" s="14">
         <v>27345</v>
       </c>
-      <c r="I81" s="15">
+      <c r="I81" s="14">
         <v>26954</v>
       </c>
-      <c r="J81" s="15">
+      <c r="J81" s="14">
         <v>26469</v>
       </c>
-      <c r="K81" s="15">
+      <c r="K81" s="14">
         <v>25957</v>
       </c>
-      <c r="L81" s="15">
+      <c r="L81" s="14">
         <v>25449</v>
       </c>
-      <c r="M81" s="15">
+      <c r="M81" s="14">
         <v>24961</v>
       </c>
-      <c r="N81" s="15">
+      <c r="N81" s="14">
         <v>24484</v>
       </c>
-      <c r="O81" s="15">
+      <c r="O81" s="14">
         <v>24005</v>
       </c>
-      <c r="P81" s="15">
+      <c r="P81" s="14">
         <v>23532</v>
       </c>
-      <c r="Q81" s="15">
+      <c r="Q81" s="14">
         <v>23067</v>
       </c>
-      <c r="R81" s="13"/>
+      <c r="R81" s="12"/>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="16">
+      <c r="B82" s="15">
         <v>32855.014999999999</v>
       </c>
-      <c r="C82" s="16">
+      <c r="C82" s="15">
         <v>34961.307999999997</v>
       </c>
-      <c r="D82" s="16">
+      <c r="D82" s="15">
         <v>37359.339</v>
       </c>
-      <c r="E82" s="16">
+      <c r="E82" s="15">
         <v>39724.885999999999</v>
       </c>
-      <c r="F82" s="16">
+      <c r="F82" s="15">
         <v>41682.067000000003</v>
       </c>
-      <c r="G82" s="16">
+      <c r="G82" s="15">
         <v>43188.125</v>
       </c>
-      <c r="H82" s="16">
+      <c r="H82" s="15">
         <v>44060.214999999997</v>
       </c>
-      <c r="I82" s="16">
+      <c r="I82" s="15">
         <v>44605.148999999998</v>
       </c>
-      <c r="J82" s="16">
+      <c r="J82" s="15">
         <v>45256.482000000004</v>
       </c>
-      <c r="K82" s="16">
+      <c r="K82" s="15">
         <v>45982.188000000002</v>
       </c>
-      <c r="L82" s="16">
+      <c r="L82" s="15">
         <v>46554.873</v>
       </c>
-      <c r="M82" s="16">
+      <c r="M82" s="15">
         <v>46609.341999999997</v>
       </c>
-      <c r="N82" s="16">
+      <c r="N82" s="15">
         <v>46346.574000000001</v>
       </c>
-      <c r="O82" s="16">
+      <c r="O82" s="15">
         <v>46044.322999999997</v>
       </c>
-      <c r="P82" s="16">
+      <c r="P82" s="15">
         <v>45725.483</v>
       </c>
-      <c r="Q82" s="16">
+      <c r="Q82" s="15">
         <v>45365.305</v>
       </c>
-      <c r="R82" s="13"/>
+      <c r="R82" s="12"/>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B83" s="14">
+      <c r="B83" s="13">
         <f>SUM(B81:B82)</f>
         <v>60554.014999999999</v>
       </c>
-      <c r="C83" s="14">
+      <c r="C83" s="13">
         <f t="shared" ref="C83:Q83" si="4">SUM(C81:C82)</f>
         <v>63313.307999999997</v>
       </c>
-      <c r="D83" s="14">
+      <c r="D83" s="13">
         <f t="shared" si="4"/>
         <v>65757.339000000007</v>
       </c>
-      <c r="E83" s="14">
+      <c r="E83" s="13">
         <f t="shared" si="4"/>
         <v>67850.885999999999</v>
       </c>
-      <c r="F83" s="14">
+      <c r="F83" s="13">
         <f t="shared" si="4"/>
         <v>69555.06700000001</v>
       </c>
-      <c r="G83" s="14">
+      <c r="G83" s="13">
         <f t="shared" si="4"/>
         <v>70822.125</v>
       </c>
-      <c r="H83" s="14">
+      <c r="H83" s="13">
         <f t="shared" si="4"/>
         <v>71405.214999999997</v>
       </c>
-      <c r="I83" s="14">
+      <c r="I83" s="13">
         <f t="shared" si="4"/>
         <v>71559.149000000005</v>
       </c>
-      <c r="J83" s="14">
+      <c r="J83" s="13">
         <f t="shared" si="4"/>
         <v>71725.482000000004</v>
       </c>
-      <c r="K83" s="14">
+      <c r="K83" s="13">
         <f t="shared" si="4"/>
         <v>71939.187999999995</v>
       </c>
-      <c r="L83" s="14">
+      <c r="L83" s="13">
         <f t="shared" si="4"/>
         <v>72003.872999999992</v>
       </c>
-      <c r="M83" s="14">
+      <c r="M83" s="13">
         <f t="shared" si="4"/>
         <v>71570.342000000004</v>
       </c>
-      <c r="N83" s="14">
+      <c r="N83" s="13">
         <f t="shared" si="4"/>
         <v>70830.573999999993</v>
       </c>
-      <c r="O83" s="14">
+      <c r="O83" s="13">
         <f t="shared" si="4"/>
         <v>70049.323000000004</v>
       </c>
-      <c r="P83" s="14">
+      <c r="P83" s="13">
         <f t="shared" si="4"/>
         <v>69257.483000000007</v>
       </c>
-      <c r="Q83" s="14">
+      <c r="Q83" s="13">
         <f t="shared" si="4"/>
         <v>68432.304999999993</v>
       </c>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A85" s="27"/>
+      <c r="A85" s="19"/>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A86" s="35" t="s">
+      <c r="A86" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="B86" s="35"/>
-      <c r="C86" s="35"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="35"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -8206,13 +8216,13 @@
       <c r="A87" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="30"/>
-      <c r="G87" s="30"/>
-      <c r="H87" s="30"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="22"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -8237,13 +8247,13 @@
       <c r="A88" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B88" s="30"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="30"/>
-      <c r="G88" s="30"/>
-      <c r="H88" s="30"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+      <c r="H88" s="22"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
@@ -8265,13 +8275,13 @@
       <c r="AA88" s="1"/>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A89" s="31" t="s">
+      <c r="A89" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B89" s="30"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
@@ -8296,67 +8306,67 @@
       <c r="AA89" s="1"/>
     </row>
     <row r="90" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A90" s="32"/>
-      <c r="B90" s="32" t="s">
+      <c r="A90" s="24"/>
+      <c r="B90" s="24" t="s">
         <v>56</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D90" s="33" t="s">
+      <c r="D90" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E90" s="33" t="s">
+      <c r="E90" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="F90" s="32" t="s">
+      <c r="F90" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="G90" s="29"/>
-      <c r="H90" s="33" t="s">
+      <c r="G90" s="21"/>
+      <c r="H90" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="I90" s="36" t="s">
+      <c r="I90" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="J90" s="36"/>
-      <c r="K90" s="29"/>
-      <c r="L90" s="29"/>
-      <c r="M90" s="29"/>
-      <c r="P90" s="29"/>
+      <c r="J90" s="37"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="21"/>
+      <c r="P90" s="21"/>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A91" s="7"/>
-      <c r="B91" s="45">
+      <c r="B91" s="35">
         <v>1996</v>
       </c>
-      <c r="C91" s="45">
+      <c r="C91" s="35">
         <v>2001</v>
       </c>
-      <c r="D91" s="45">
+      <c r="D91" s="35">
         <v>2011</v>
       </c>
-      <c r="E91" s="45">
+      <c r="E91" s="35">
         <v>2016</v>
       </c>
-      <c r="F91" s="45">
+      <c r="F91" s="35">
         <v>2019</v>
       </c>
-      <c r="G91" s="28"/>
+      <c r="G91" s="20"/>
       <c r="H91" s="7"/>
-      <c r="I91" s="37">
+      <c r="I91" s="27">
         <v>1996</v>
       </c>
       <c r="J91" s="7">
         <v>2019</v>
       </c>
-      <c r="K91" s="28"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="28"/>
-      <c r="P91" s="28"/>
+      <c r="K91" s="20"/>
+      <c r="L91" s="20"/>
+      <c r="M91" s="20"/>
+      <c r="P91" s="20"/>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B92" s="4">
@@ -8374,20 +8384,20 @@
       <c r="F92" s="4">
         <v>624531</v>
       </c>
-      <c r="G92" s="27"/>
+      <c r="G92" s="19"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
       <c r="J92" s="4">
         <f>47443259-322416</f>
         <v>47120843</v>
       </c>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="M92" s="27"/>
-      <c r="P92" s="27"/>
+      <c r="K92" s="19"/>
+      <c r="L92" s="19"/>
+      <c r="M92" s="19"/>
+      <c r="P92" s="19"/>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A93" s="17" t="s">
+      <c r="A93" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B93" s="4">
@@ -8405,20 +8415,20 @@
       <c r="F93" s="4">
         <v>607157</v>
       </c>
-      <c r="G93" s="27"/>
+      <c r="G93" s="19"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
       <c r="J93" s="4">
         <f>5176750-42971</f>
         <v>5133779</v>
       </c>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
-      <c r="M93" s="27"/>
-      <c r="P93" s="27"/>
+      <c r="K93" s="19"/>
+      <c r="L93" s="19"/>
+      <c r="M93" s="19"/>
+      <c r="P93" s="19"/>
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B94" s="4">
@@ -8436,20 +8446,20 @@
       <c r="F94" s="4">
         <v>573074</v>
       </c>
-      <c r="G94" s="27"/>
+      <c r="G94" s="19"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
       <c r="J94" s="4">
         <f>1503007-21608</f>
         <v>1481399</v>
       </c>
-      <c r="K94" s="27"/>
-      <c r="L94" s="27"/>
-      <c r="M94" s="27"/>
-      <c r="P94" s="27"/>
+      <c r="K94" s="19"/>
+      <c r="L94" s="19"/>
+      <c r="M94" s="19"/>
+      <c r="P94" s="19"/>
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B95" s="4">
@@ -8467,20 +8477,20 @@
       <c r="F95" s="4">
         <v>492961</v>
       </c>
-      <c r="G95" s="27"/>
+      <c r="G95" s="19"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
       <c r="J95" s="4">
         <f>4652006-215973</f>
         <v>4436033</v>
       </c>
-      <c r="K95" s="27"/>
-      <c r="L95" s="27"/>
-      <c r="M95" s="27"/>
-      <c r="P95" s="27"/>
+      <c r="K95" s="19"/>
+      <c r="L95" s="19"/>
+      <c r="M95" s="19"/>
+      <c r="P95" s="19"/>
     </row>
     <row r="96" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A96" s="17" t="s">
+      <c r="A96" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B96" s="4">
@@ -8498,8 +8508,8 @@
       <c r="F96" s="4">
         <v>505198</v>
       </c>
-      <c r="G96" s="27"/>
-      <c r="H96" s="38" t="s">
+      <c r="G96" s="19"/>
+      <c r="H96" s="28" t="s">
         <v>64</v>
       </c>
       <c r="I96" s="4">
@@ -8510,13 +8520,13 @@
         <f>SUM(J92:J95)</f>
         <v>58172054</v>
       </c>
-      <c r="K96" s="27"/>
-      <c r="L96" s="27"/>
-      <c r="M96" s="27"/>
-      <c r="P96" s="27"/>
+      <c r="K96" s="19"/>
+      <c r="L96" s="19"/>
+      <c r="M96" s="19"/>
+      <c r="P96" s="19"/>
     </row>
     <row r="97" spans="1:17" ht="58" x14ac:dyDescent="0.35">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B97" s="4">
@@ -8534,8 +8544,8 @@
       <c r="F97" s="4">
         <v>534838</v>
       </c>
-      <c r="G97" s="27"/>
-      <c r="H97" s="38" t="s">
+      <c r="G97" s="19"/>
+      <c r="H97" s="28" t="s">
         <v>65</v>
       </c>
       <c r="I97" s="4">
@@ -8546,13 +8556,13 @@
         <f>J96/1000</f>
         <v>58172.053999999996</v>
       </c>
-      <c r="K97" s="27"/>
-      <c r="L97" s="27"/>
-      <c r="M97" s="27"/>
-      <c r="P97" s="27"/>
+      <c r="K97" s="19"/>
+      <c r="L97" s="19"/>
+      <c r="M97" s="19"/>
+      <c r="P97" s="19"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B98" s="4">
@@ -8570,18 +8580,18 @@
       <c r="F98" s="4">
         <v>505101</v>
       </c>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
-      <c r="P98" s="27"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="19"/>
+      <c r="I98" s="19"/>
+      <c r="J98" s="19"/>
+      <c r="K98" s="19"/>
+      <c r="L98" s="19"/>
+      <c r="M98" s="19"/>
+      <c r="N98" s="19"/>
+      <c r="P98" s="19"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B99" s="4">
@@ -8599,19 +8609,19 @@
       <c r="F99" s="4">
         <v>392259</v>
       </c>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="27"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="27"/>
-      <c r="M99" s="27"/>
-      <c r="N99" s="27"/>
-      <c r="O99" s="27"/>
-      <c r="P99" s="27"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="19"/>
+      <c r="I99" s="19"/>
+      <c r="J99" s="19"/>
+      <c r="K99" s="19"/>
+      <c r="L99" s="19"/>
+      <c r="M99" s="19"/>
+      <c r="N99" s="19"/>
+      <c r="O99" s="19"/>
+      <c r="P99" s="19"/>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A100" s="17" t="s">
+      <c r="A100" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B100" s="4">
@@ -8629,19 +8639,19 @@
       <c r="F100" s="4">
         <v>282544</v>
       </c>
-      <c r="G100" s="27"/>
-      <c r="H100" s="27"/>
-      <c r="I100" s="27"/>
-      <c r="J100" s="27"/>
-      <c r="K100" s="27"/>
-      <c r="L100" s="27"/>
-      <c r="M100" s="27"/>
-      <c r="N100" s="27"/>
-      <c r="O100" s="27"/>
-      <c r="P100" s="27"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="19"/>
+      <c r="I100" s="19"/>
+      <c r="J100" s="19"/>
+      <c r="K100" s="19"/>
+      <c r="L100" s="19"/>
+      <c r="M100" s="19"/>
+      <c r="N100" s="19"/>
+      <c r="O100" s="19"/>
+      <c r="P100" s="19"/>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A101" s="17" t="s">
+      <c r="A101" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B101" s="4">
@@ -8659,19 +8669,19 @@
       <c r="F101" s="4">
         <v>226914</v>
       </c>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="27"/>
-      <c r="K101" s="27"/>
-      <c r="L101" s="27"/>
-      <c r="M101" s="27"/>
-      <c r="N101" s="27"/>
-      <c r="O101" s="27"/>
-      <c r="P101" s="27"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="19"/>
+      <c r="I101" s="19"/>
+      <c r="J101" s="19"/>
+      <c r="K101" s="19"/>
+      <c r="L101" s="19"/>
+      <c r="M101" s="19"/>
+      <c r="N101" s="19"/>
+      <c r="O101" s="19"/>
+      <c r="P101" s="19"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A102" s="17" t="s">
+      <c r="A102" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B102" s="4">
@@ -8689,19 +8699,19 @@
       <c r="F102" s="4">
         <v>168558</v>
       </c>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
-      <c r="J102" s="27"/>
-      <c r="K102" s="27"/>
-      <c r="L102" s="27"/>
-      <c r="M102" s="27"/>
-      <c r="N102" s="27"/>
-      <c r="O102" s="27"/>
-      <c r="P102" s="27"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
+      <c r="M102" s="19"/>
+      <c r="N102" s="19"/>
+      <c r="O102" s="19"/>
+      <c r="P102" s="19"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A103" s="17" t="s">
+      <c r="A103" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B103" s="4">
@@ -8719,19 +8729,19 @@
       <c r="F103" s="4">
         <v>143386</v>
       </c>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="27"/>
-      <c r="K103" s="27"/>
-      <c r="L103" s="27"/>
-      <c r="M103" s="27"/>
-      <c r="N103" s="27"/>
-      <c r="O103" s="27"/>
-      <c r="P103" s="27"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+      <c r="J103" s="19"/>
+      <c r="K103" s="19"/>
+      <c r="L103" s="19"/>
+      <c r="M103" s="19"/>
+      <c r="N103" s="19"/>
+      <c r="O103" s="19"/>
+      <c r="P103" s="19"/>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A104" s="17" t="s">
+      <c r="A104" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B104" s="4">
@@ -8749,19 +8759,19 @@
       <c r="F104" s="4">
         <v>114078</v>
       </c>
-      <c r="G104" s="27"/>
-      <c r="H104" s="27"/>
-      <c r="I104" s="27"/>
-      <c r="J104" s="27"/>
-      <c r="K104" s="27"/>
-      <c r="L104" s="27"/>
-      <c r="M104" s="27"/>
-      <c r="N104" s="27"/>
-      <c r="O104" s="27"/>
-      <c r="P104" s="27"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
+      <c r="K104" s="19"/>
+      <c r="L104" s="19"/>
+      <c r="M104" s="19"/>
+      <c r="N104" s="19"/>
+      <c r="O104" s="19"/>
+      <c r="P104" s="19"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A105" s="17" t="s">
+      <c r="A105" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B105" s="4">
@@ -8779,19 +8789,19 @@
       <c r="F105" s="4">
         <v>89431</v>
       </c>
-      <c r="G105" s="27"/>
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="27"/>
-      <c r="K105" s="27"/>
-      <c r="L105" s="27"/>
-      <c r="M105" s="27"/>
-      <c r="N105" s="27"/>
-      <c r="O105" s="27"/>
-      <c r="P105" s="27"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="19"/>
+      <c r="J105" s="19"/>
+      <c r="K105" s="19"/>
+      <c r="L105" s="19"/>
+      <c r="M105" s="19"/>
+      <c r="N105" s="19"/>
+      <c r="O105" s="19"/>
+      <c r="P105" s="19"/>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A106" s="17" t="s">
+      <c r="A106" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B106" s="4">
@@ -8809,20 +8819,20 @@
       <c r="F106" s="4">
         <v>60742</v>
       </c>
-      <c r="G106" s="27"/>
-      <c r="H106" s="27"/>
-      <c r="I106" s="27"/>
-      <c r="J106" s="27"/>
-      <c r="K106" s="27"/>
-      <c r="L106" s="27"/>
-      <c r="M106" s="27"/>
-      <c r="N106" s="27"/>
-      <c r="O106" s="27"/>
-      <c r="P106" s="27"/>
-      <c r="Q106" s="27"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="19"/>
+      <c r="L106" s="19"/>
+      <c r="M106" s="19"/>
+      <c r="N106" s="19"/>
+      <c r="O106" s="19"/>
+      <c r="P106" s="19"/>
+      <c r="Q106" s="19"/>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A107" s="17" t="s">
+      <c r="A107" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B107" s="4">
@@ -8840,20 +8850,20 @@
       <c r="F107" s="4">
         <v>34596</v>
       </c>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="27"/>
-      <c r="L107" s="27"/>
-      <c r="M107" s="27"/>
-      <c r="N107" s="27"/>
-      <c r="O107" s="27"/>
-      <c r="P107" s="27"/>
-      <c r="Q107" s="27"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+      <c r="M107" s="19"/>
+      <c r="N107" s="19"/>
+      <c r="O107" s="19"/>
+      <c r="P107" s="19"/>
+      <c r="Q107" s="19"/>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A108" s="18" t="s">
+      <c r="A108" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B108">
@@ -8876,56 +8886,56 @@
         <f>SUM(F92:F105)</f>
         <v>5260030</v>
       </c>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
-      <c r="I108" s="27"/>
-      <c r="J108" s="27"/>
-      <c r="K108" s="27"/>
-      <c r="L108" s="27"/>
-      <c r="M108" s="27"/>
-      <c r="N108" s="27"/>
-      <c r="O108" s="27"/>
-      <c r="P108" s="27"/>
-      <c r="Q108" s="27"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
+      <c r="J108" s="19"/>
+      <c r="K108" s="19"/>
+      <c r="L108" s="19"/>
+      <c r="M108" s="19"/>
+      <c r="N108" s="19"/>
+      <c r="O108" s="19"/>
+      <c r="P108" s="19"/>
+      <c r="Q108" s="19"/>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="27"/>
-      <c r="L109" s="27"/>
-      <c r="M109" s="27"/>
-      <c r="N109" s="27"/>
-      <c r="O109" s="27"/>
-      <c r="P109" s="27"/>
-      <c r="Q109" s="27"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
+      <c r="J109" s="19"/>
+      <c r="K109" s="19"/>
+      <c r="L109" s="19"/>
+      <c r="M109" s="19"/>
+      <c r="N109" s="19"/>
+      <c r="O109" s="19"/>
+      <c r="P109" s="19"/>
+      <c r="Q109" s="19"/>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A110" s="32"/>
-      <c r="B110" s="32" t="s">
+      <c r="A110" s="24"/>
+      <c r="B110" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C110" s="32" t="s">
+      <c r="C110" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D110" s="32"/>
+      <c r="D110" s="24"/>
       <c r="E110" s="4"/>
-      <c r="F110" s="32" t="s">
+      <c r="F110" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="G110" s="29"/>
-      <c r="H110" s="29"/>
-      <c r="I110" s="29"/>
-      <c r="J110" s="29"/>
-      <c r="K110" s="29"/>
-      <c r="L110" s="29"/>
-      <c r="M110" s="29"/>
-      <c r="N110" s="29"/>
-      <c r="O110" s="29"/>
-      <c r="P110" s="29"/>
-      <c r="Q110" s="27"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+      <c r="J110" s="21"/>
+      <c r="K110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="21"/>
+      <c r="N110" s="21"/>
+      <c r="O110" s="21"/>
+      <c r="P110" s="21"/>
+      <c r="Q110" s="19"/>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="7"/>
@@ -8944,20 +8954,20 @@
       <c r="F111" s="7">
         <v>2019</v>
       </c>
-      <c r="G111" s="28"/>
-      <c r="H111" s="28"/>
-      <c r="I111" s="28"/>
-      <c r="J111" s="28"/>
-      <c r="K111" s="28"/>
-      <c r="L111" s="28"/>
-      <c r="M111" s="28"/>
-      <c r="N111" s="28"/>
-      <c r="O111" s="28"/>
-      <c r="P111" s="28"/>
-      <c r="Q111" s="27"/>
+      <c r="G111" s="20"/>
+      <c r="H111" s="20"/>
+      <c r="I111" s="20"/>
+      <c r="J111" s="20"/>
+      <c r="K111" s="20"/>
+      <c r="L111" s="20"/>
+      <c r="M111" s="20"/>
+      <c r="N111" s="20"/>
+      <c r="O111" s="20"/>
+      <c r="P111" s="20"/>
+      <c r="Q111" s="19"/>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A112" s="17" t="s">
+      <c r="A112" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B112" s="4">
@@ -8971,19 +8981,19 @@
       <c r="F112" s="4">
         <v>606570</v>
       </c>
-      <c r="G112" s="27"/>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-      <c r="J112" s="27"/>
-      <c r="K112" s="27"/>
-      <c r="L112" s="27"/>
-      <c r="M112" s="27"/>
-      <c r="N112" s="27"/>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
+      <c r="K112" s="19"/>
+      <c r="L112" s="19"/>
+      <c r="M112" s="19"/>
+      <c r="N112" s="19"/>
+      <c r="O112" s="19"/>
+      <c r="P112" s="19"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A113" s="17" t="s">
+      <c r="A113" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B113" s="4">
@@ -8997,19 +9007,19 @@
       <c r="F113" s="4">
         <v>589752</v>
       </c>
-      <c r="G113" s="27"/>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="27"/>
-      <c r="K113" s="27"/>
-      <c r="L113" s="27"/>
-      <c r="M113" s="27"/>
-      <c r="N113" s="27"/>
-      <c r="O113" s="27"/>
-      <c r="P113" s="27"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19"/>
+      <c r="I113" s="19"/>
+      <c r="J113" s="19"/>
+      <c r="K113" s="19"/>
+      <c r="L113" s="19"/>
+      <c r="M113" s="19"/>
+      <c r="N113" s="19"/>
+      <c r="O113" s="19"/>
+      <c r="P113" s="19"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A114" s="17" t="s">
+      <c r="A114" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B114" s="4">
@@ -9023,19 +9033,19 @@
       <c r="F114" s="4">
         <v>563089</v>
       </c>
-      <c r="G114" s="27"/>
-      <c r="H114" s="27"/>
-      <c r="I114" s="27"/>
-      <c r="J114" s="27"/>
-      <c r="K114" s="27"/>
-      <c r="L114" s="27"/>
-      <c r="M114" s="27"/>
-      <c r="N114" s="27"/>
-      <c r="O114" s="27"/>
-      <c r="P114" s="27"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="19"/>
+      <c r="I114" s="19"/>
+      <c r="J114" s="19"/>
+      <c r="K114" s="19"/>
+      <c r="L114" s="19"/>
+      <c r="M114" s="19"/>
+      <c r="N114" s="19"/>
+      <c r="O114" s="19"/>
+      <c r="P114" s="19"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A115" s="17" t="s">
+      <c r="A115" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B115" s="4">
@@ -9049,19 +9059,19 @@
       <c r="F115" s="4">
         <v>487612</v>
       </c>
-      <c r="G115" s="27"/>
-      <c r="H115" s="27"/>
-      <c r="I115" s="27"/>
-      <c r="J115" s="27"/>
-      <c r="K115" s="27"/>
-      <c r="L115" s="27"/>
-      <c r="M115" s="27"/>
-      <c r="N115" s="27"/>
-      <c r="O115" s="27"/>
-      <c r="P115" s="27"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="19"/>
+      <c r="I115" s="19"/>
+      <c r="J115" s="19"/>
+      <c r="K115" s="19"/>
+      <c r="L115" s="19"/>
+      <c r="M115" s="19"/>
+      <c r="N115" s="19"/>
+      <c r="O115" s="19"/>
+      <c r="P115" s="19"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A116" s="17" t="s">
+      <c r="A116" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B116" s="4">
@@ -9075,19 +9085,19 @@
       <c r="F116" s="4">
         <v>500833</v>
       </c>
-      <c r="G116" s="27"/>
-      <c r="H116" s="27"/>
-      <c r="I116" s="27"/>
-      <c r="J116" s="27"/>
-      <c r="K116" s="27"/>
-      <c r="L116" s="27"/>
-      <c r="M116" s="27"/>
-      <c r="N116" s="27"/>
-      <c r="O116" s="27"/>
-      <c r="P116" s="27"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="19"/>
+      <c r="I116" s="19"/>
+      <c r="J116" s="19"/>
+      <c r="K116" s="19"/>
+      <c r="L116" s="19"/>
+      <c r="M116" s="19"/>
+      <c r="N116" s="19"/>
+      <c r="O116" s="19"/>
+      <c r="P116" s="19"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A117" s="17" t="s">
+      <c r="A117" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B117" s="4">
@@ -9101,19 +9111,19 @@
       <c r="F117" s="4">
         <v>526234</v>
       </c>
-      <c r="G117" s="27"/>
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
-      <c r="J117" s="27"/>
-      <c r="K117" s="27"/>
-      <c r="L117" s="27"/>
-      <c r="M117" s="27"/>
-      <c r="N117" s="27"/>
-      <c r="O117" s="27"/>
-      <c r="P117" s="27"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="19"/>
+      <c r="I117" s="19"/>
+      <c r="J117" s="19"/>
+      <c r="K117" s="19"/>
+      <c r="L117" s="19"/>
+      <c r="M117" s="19"/>
+      <c r="N117" s="19"/>
+      <c r="O117" s="19"/>
+      <c r="P117" s="19"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A118" s="17" t="s">
+      <c r="A118" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B118" s="4">
@@ -9127,19 +9137,19 @@
       <c r="F118" s="4">
         <v>503472</v>
       </c>
-      <c r="G118" s="27"/>
-      <c r="H118" s="27"/>
-      <c r="I118" s="27"/>
-      <c r="J118" s="27"/>
-      <c r="K118" s="27"/>
-      <c r="L118" s="27"/>
-      <c r="M118" s="27"/>
-      <c r="N118" s="27"/>
-      <c r="O118" s="27"/>
-      <c r="P118" s="27"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="19"/>
+      <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="19"/>
+      <c r="L118" s="19"/>
+      <c r="M118" s="19"/>
+      <c r="N118" s="19"/>
+      <c r="O118" s="19"/>
+      <c r="P118" s="19"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A119" s="17" t="s">
+      <c r="A119" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B119" s="4">
@@ -9153,19 +9163,19 @@
       <c r="F119" s="4">
         <v>413146</v>
       </c>
-      <c r="G119" s="27"/>
-      <c r="H119" s="27"/>
-      <c r="I119" s="27"/>
-      <c r="J119" s="27"/>
-      <c r="K119" s="27"/>
-      <c r="L119" s="27"/>
-      <c r="M119" s="27"/>
-      <c r="N119" s="27"/>
-      <c r="O119" s="27"/>
-      <c r="P119" s="27"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="19"/>
+      <c r="I119" s="19"/>
+      <c r="J119" s="19"/>
+      <c r="K119" s="19"/>
+      <c r="L119" s="19"/>
+      <c r="M119" s="19"/>
+      <c r="N119" s="19"/>
+      <c r="O119" s="19"/>
+      <c r="P119" s="19"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A120" s="17" t="s">
+      <c r="A120" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B120" s="4">
@@ -9179,19 +9189,19 @@
       <c r="F120" s="4">
         <v>330508</v>
       </c>
-      <c r="G120" s="27"/>
-      <c r="H120" s="27"/>
-      <c r="I120" s="27"/>
-      <c r="J120" s="27"/>
-      <c r="K120" s="27"/>
-      <c r="L120" s="27"/>
-      <c r="M120" s="27"/>
-      <c r="N120" s="27"/>
-      <c r="O120" s="27"/>
-      <c r="P120" s="27"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="19"/>
+      <c r="I120" s="19"/>
+      <c r="J120" s="19"/>
+      <c r="K120" s="19"/>
+      <c r="L120" s="19"/>
+      <c r="M120" s="19"/>
+      <c r="N120" s="19"/>
+      <c r="O120" s="19"/>
+      <c r="P120" s="19"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A121" s="17" t="s">
+      <c r="A121" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B121" s="4">
@@ -9205,19 +9215,19 @@
       <c r="F121" s="4">
         <v>290118</v>
       </c>
-      <c r="G121" s="27"/>
-      <c r="H121" s="27"/>
-      <c r="I121" s="27"/>
-      <c r="J121" s="27"/>
-      <c r="K121" s="27"/>
-      <c r="L121" s="27"/>
-      <c r="M121" s="27"/>
-      <c r="N121" s="27"/>
-      <c r="O121" s="27"/>
-      <c r="P121" s="27"/>
+      <c r="G121" s="19"/>
+      <c r="H121" s="19"/>
+      <c r="I121" s="19"/>
+      <c r="J121" s="19"/>
+      <c r="K121" s="19"/>
+      <c r="L121" s="19"/>
+      <c r="M121" s="19"/>
+      <c r="N121" s="19"/>
+      <c r="O121" s="19"/>
+      <c r="P121" s="19"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A122" s="17" t="s">
+      <c r="A122" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B122" s="4">
@@ -9231,19 +9241,19 @@
       <c r="F122" s="4">
         <v>255374</v>
       </c>
-      <c r="G122" s="27"/>
-      <c r="H122" s="27"/>
-      <c r="I122" s="27"/>
-      <c r="J122" s="27"/>
-      <c r="K122" s="27"/>
-      <c r="L122" s="27"/>
-      <c r="M122" s="27"/>
-      <c r="N122" s="27"/>
-      <c r="O122" s="27"/>
-      <c r="P122" s="27"/>
+      <c r="G122" s="19"/>
+      <c r="H122" s="19"/>
+      <c r="I122" s="19"/>
+      <c r="J122" s="19"/>
+      <c r="K122" s="19"/>
+      <c r="L122" s="19"/>
+      <c r="M122" s="19"/>
+      <c r="N122" s="19"/>
+      <c r="O122" s="19"/>
+      <c r="P122" s="19"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A123" s="17" t="s">
+      <c r="A123" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B123" s="4">
@@ -9257,19 +9267,19 @@
       <c r="F123" s="4">
         <v>233152</v>
       </c>
-      <c r="G123" s="27"/>
-      <c r="H123" s="27"/>
-      <c r="I123" s="27"/>
-      <c r="J123" s="27"/>
-      <c r="K123" s="27"/>
-      <c r="L123" s="27"/>
-      <c r="M123" s="27"/>
-      <c r="N123" s="27"/>
-      <c r="O123" s="27"/>
-      <c r="P123" s="27"/>
+      <c r="G123" s="19"/>
+      <c r="H123" s="19"/>
+      <c r="I123" s="19"/>
+      <c r="J123" s="19"/>
+      <c r="K123" s="19"/>
+      <c r="L123" s="19"/>
+      <c r="M123" s="19"/>
+      <c r="N123" s="19"/>
+      <c r="O123" s="19"/>
+      <c r="P123" s="19"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A124" s="17" t="s">
+      <c r="A124" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B124" s="4">
@@ -9283,19 +9293,19 @@
       <c r="F124" s="4">
         <v>192451</v>
       </c>
-      <c r="G124" s="27"/>
-      <c r="H124" s="27"/>
-      <c r="I124" s="27"/>
-      <c r="J124" s="27"/>
-      <c r="K124" s="27"/>
-      <c r="L124" s="27"/>
-      <c r="M124" s="27"/>
-      <c r="N124" s="27"/>
-      <c r="O124" s="27"/>
-      <c r="P124" s="27"/>
+      <c r="G124" s="19"/>
+      <c r="H124" s="19"/>
+      <c r="I124" s="19"/>
+      <c r="J124" s="19"/>
+      <c r="K124" s="19"/>
+      <c r="L124" s="19"/>
+      <c r="M124" s="19"/>
+      <c r="N124" s="19"/>
+      <c r="O124" s="19"/>
+      <c r="P124" s="19"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A125" s="17" t="s">
+      <c r="A125" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B125" s="4">
@@ -9309,19 +9319,19 @@
       <c r="F125" s="4">
         <v>155433</v>
       </c>
-      <c r="G125" s="27"/>
-      <c r="H125" s="27"/>
-      <c r="I125" s="27"/>
-      <c r="J125" s="27"/>
-      <c r="K125" s="27"/>
-      <c r="L125" s="27"/>
-      <c r="M125" s="27"/>
-      <c r="N125" s="27"/>
-      <c r="O125" s="27"/>
-      <c r="P125" s="27"/>
+      <c r="G125" s="19"/>
+      <c r="H125" s="19"/>
+      <c r="I125" s="19"/>
+      <c r="J125" s="19"/>
+      <c r="K125" s="19"/>
+      <c r="L125" s="19"/>
+      <c r="M125" s="19"/>
+      <c r="N125" s="19"/>
+      <c r="O125" s="19"/>
+      <c r="P125" s="19"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A126" s="17" t="s">
+      <c r="A126" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B126" s="4">
@@ -9335,19 +9345,19 @@
       <c r="F126" s="4">
         <v>118042</v>
       </c>
-      <c r="G126" s="27"/>
-      <c r="H126" s="27"/>
-      <c r="I126" s="27"/>
-      <c r="J126" s="27"/>
-      <c r="K126" s="27"/>
-      <c r="L126" s="27"/>
-      <c r="M126" s="27"/>
-      <c r="N126" s="27"/>
-      <c r="O126" s="27"/>
-      <c r="P126" s="27"/>
+      <c r="G126" s="19"/>
+      <c r="H126" s="19"/>
+      <c r="I126" s="19"/>
+      <c r="J126" s="19"/>
+      <c r="K126" s="19"/>
+      <c r="L126" s="19"/>
+      <c r="M126" s="19"/>
+      <c r="N126" s="19"/>
+      <c r="O126" s="19"/>
+      <c r="P126" s="19"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A127" s="17" t="s">
+      <c r="A127" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B127" s="4">
@@ -9361,19 +9371,19 @@
       <c r="F127" s="4">
         <v>71508</v>
       </c>
-      <c r="G127" s="27"/>
-      <c r="H127" s="27"/>
-      <c r="I127" s="27"/>
-      <c r="J127" s="27"/>
-      <c r="K127" s="27"/>
-      <c r="L127" s="27"/>
-      <c r="M127" s="27"/>
-      <c r="N127" s="27"/>
-      <c r="O127" s="27"/>
-      <c r="P127" s="27"/>
+      <c r="G127" s="19"/>
+      <c r="H127" s="19"/>
+      <c r="I127" s="19"/>
+      <c r="J127" s="19"/>
+      <c r="K127" s="19"/>
+      <c r="L127" s="19"/>
+      <c r="M127" s="19"/>
+      <c r="N127" s="19"/>
+      <c r="O127" s="19"/>
+      <c r="P127" s="19"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A128" s="18" t="s">
+      <c r="A128" s="17" t="s">
         <v>60</v>
       </c>
       <c r="B128">
@@ -9394,19 +9404,19 @@
         <f t="shared" si="5"/>
         <v>5647744</v>
       </c>
-      <c r="G128" s="27"/>
-      <c r="H128" s="27"/>
-      <c r="I128" s="27"/>
-      <c r="J128" s="27"/>
-      <c r="K128" s="27"/>
-      <c r="L128" s="27"/>
-      <c r="M128" s="27"/>
-      <c r="N128" s="27"/>
-      <c r="O128" s="27"/>
-      <c r="P128" s="27"/>
+      <c r="G128" s="19"/>
+      <c r="H128" s="19"/>
+      <c r="I128" s="19"/>
+      <c r="J128" s="19"/>
+      <c r="K128" s="19"/>
+      <c r="L128" s="19"/>
+      <c r="M128" s="19"/>
+      <c r="N128" s="19"/>
+      <c r="O128" s="19"/>
+      <c r="P128" s="19"/>
     </row>
     <row r="129" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A129" s="34" t="s">
+      <c r="A129" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B129">
@@ -9431,7 +9441,7 @@
       </c>
     </row>
     <row r="130" spans="1:19" ht="58" x14ac:dyDescent="0.35">
-      <c r="A130" s="34" t="s">
+      <c r="A130" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B130" s="1">
@@ -9456,100 +9466,100 @@
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A133" s="35" t="s">
+      <c r="A133" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="B133" s="35"/>
-      <c r="C133" s="35"/>
-      <c r="D133" s="35"/>
-      <c r="E133" s="35"/>
-      <c r="F133" s="35"/>
-      <c r="G133" s="35"/>
-      <c r="H133" s="35"/>
+      <c r="B133" s="38"/>
+      <c r="C133" s="38"/>
+      <c r="D133" s="38"/>
+      <c r="E133" s="38"/>
+      <c r="F133" s="38"/>
+      <c r="G133" s="38"/>
+      <c r="H133" s="38"/>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A134" s="31" t="s">
+      <c r="A134" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B134" s="30"/>
-      <c r="C134" s="30"/>
-      <c r="D134" s="30"/>
-      <c r="E134" s="30"/>
-      <c r="F134" s="30"/>
-      <c r="G134" s="30"/>
-      <c r="H134" s="30"/>
+      <c r="B134" s="22"/>
+      <c r="C134" s="22"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="22"/>
+      <c r="G134" s="22"/>
+      <c r="H134" s="22"/>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" s="4"/>
-      <c r="B135" s="32">
+      <c r="B135" s="24">
         <v>2002</v>
       </c>
-      <c r="C135" s="32">
-        <f>B135+1</f>
+      <c r="C135" s="24">
+        <f t="shared" ref="C135:S135" si="8">B135+1</f>
         <v>2003</v>
       </c>
-      <c r="D135" s="32">
-        <f>C135+1</f>
+      <c r="D135" s="24">
+        <f t="shared" si="8"/>
         <v>2004</v>
       </c>
-      <c r="E135" s="32">
-        <f>D135+1</f>
+      <c r="E135" s="24">
+        <f t="shared" si="8"/>
         <v>2005</v>
       </c>
-      <c r="F135" s="32">
-        <f>E135+1</f>
+      <c r="F135" s="24">
+        <f t="shared" si="8"/>
         <v>2006</v>
       </c>
-      <c r="G135" s="32">
-        <f>F135+1</f>
+      <c r="G135" s="24">
+        <f t="shared" si="8"/>
         <v>2007</v>
       </c>
-      <c r="H135" s="32">
-        <f>G135+1</f>
+      <c r="H135" s="24">
+        <f t="shared" si="8"/>
         <v>2008</v>
       </c>
-      <c r="I135" s="32">
-        <f>H135+1</f>
+      <c r="I135" s="24">
+        <f t="shared" si="8"/>
         <v>2009</v>
       </c>
-      <c r="J135" s="32">
-        <f>I135+1</f>
+      <c r="J135" s="24">
+        <f t="shared" si="8"/>
         <v>2010</v>
       </c>
-      <c r="K135" s="32">
-        <f>J135+1</f>
+      <c r="K135" s="24">
+        <f t="shared" si="8"/>
         <v>2011</v>
       </c>
-      <c r="L135" s="32">
-        <f>K135+1</f>
+      <c r="L135" s="24">
+        <f t="shared" si="8"/>
         <v>2012</v>
       </c>
-      <c r="M135" s="32">
-        <f>L135+1</f>
+      <c r="M135" s="24">
+        <f t="shared" si="8"/>
         <v>2013</v>
       </c>
-      <c r="N135" s="32">
-        <f>M135+1</f>
+      <c r="N135" s="24">
+        <f t="shared" si="8"/>
         <v>2014</v>
       </c>
-      <c r="O135" s="32">
-        <f>N135+1</f>
+      <c r="O135" s="24">
+        <f t="shared" si="8"/>
         <v>2015</v>
       </c>
-      <c r="P135" s="32">
-        <f>O135+1</f>
+      <c r="P135" s="24">
+        <f t="shared" si="8"/>
         <v>2016</v>
       </c>
-      <c r="Q135" s="32">
-        <f>P135+1</f>
+      <c r="Q135" s="24">
+        <f t="shared" si="8"/>
         <v>2017</v>
       </c>
-      <c r="R135" s="32">
-        <f>Q135+1</f>
+      <c r="R135" s="24">
+        <f t="shared" si="8"/>
         <v>2018</v>
       </c>
-      <c r="S135" s="32">
-        <f>R135+1</f>
+      <c r="S135" s="24">
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
     </row>
@@ -9557,58 +9567,58 @@
       <c r="A136" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B136" s="39">
+      <c r="B136" s="29">
         <v>20.8</v>
       </c>
-      <c r="C136" s="40">
+      <c r="C136" s="30">
         <v>20.7</v>
       </c>
-      <c r="D136" s="40">
+      <c r="D136" s="30">
         <v>20.6</v>
       </c>
-      <c r="E136" s="40">
+      <c r="E136" s="30">
         <v>20.5</v>
       </c>
-      <c r="F136" s="40">
+      <c r="F136" s="30">
         <v>20.399999999999999</v>
       </c>
-      <c r="G136" s="41">
+      <c r="G136" s="31">
         <v>20.3</v>
       </c>
-      <c r="H136" s="41">
+      <c r="H136" s="31">
         <v>20.2</v>
       </c>
-      <c r="I136" s="41">
+      <c r="I136" s="31">
         <v>20.100000000000001</v>
       </c>
-      <c r="J136" s="41">
+      <c r="J136" s="31">
         <v>20</v>
       </c>
-      <c r="K136" s="41">
+      <c r="K136" s="31">
         <v>19.8</v>
       </c>
-      <c r="L136" s="41">
+      <c r="L136" s="31">
         <v>19.8</v>
       </c>
-      <c r="M136" s="41">
+      <c r="M136" s="31">
         <v>19.7</v>
       </c>
-      <c r="N136" s="41">
+      <c r="N136" s="31">
         <v>19.600000000000001</v>
       </c>
-      <c r="O136" s="41">
+      <c r="O136" s="31">
         <v>19.5</v>
       </c>
-      <c r="P136" s="41">
+      <c r="P136" s="31">
         <v>19.399999999999999</v>
       </c>
-      <c r="Q136" s="42">
+      <c r="Q136" s="32">
         <v>19.3</v>
       </c>
-      <c r="R136" s="42">
+      <c r="R136" s="32">
         <v>19.3</v>
       </c>
-      <c r="S136" s="42">
+      <c r="S136" s="32">
         <v>19.2</v>
       </c>
     </row>
@@ -9621,76 +9631,76 @@
         <v>0.20800000000000002</v>
       </c>
       <c r="C137" s="4">
-        <f t="shared" ref="C137:S137" si="8">C136/100</f>
+        <f t="shared" ref="C137:S137" si="9">C136/100</f>
         <v>0.20699999999999999</v>
       </c>
       <c r="D137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20600000000000002</v>
       </c>
       <c r="E137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20499999999999999</v>
       </c>
       <c r="F137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20399999999999999</v>
       </c>
       <c r="G137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20300000000000001</v>
       </c>
       <c r="H137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20199999999999999</v>
       </c>
       <c r="I137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.20100000000000001</v>
       </c>
       <c r="J137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
       <c r="K137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19800000000000001</v>
       </c>
       <c r="L137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19800000000000001</v>
       </c>
       <c r="M137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19699999999999998</v>
       </c>
       <c r="N137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19600000000000001</v>
       </c>
       <c r="O137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="P137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.19399999999999998</v>
       </c>
       <c r="Q137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.193</v>
       </c>
       <c r="R137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.193</v>
       </c>
       <c r="S137" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.192</v>
       </c>
     </row>
     <row r="138" spans="1:19" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A138" s="43" t="s">
+      <c r="A138" s="33" t="s">
         <v>74</v>
       </c>
       <c r="E138">
@@ -9711,7 +9721,7 @@
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A139" s="43"/>
+      <c r="A139" s="33"/>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
@@ -9732,136 +9742,211 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" s="4"/>
-      <c r="B144" s="45">
+      <c r="B144" s="4"/>
+      <c r="C144" s="35">
         <v>2025</v>
       </c>
-      <c r="C144" s="45">
+      <c r="D144" s="35">
         <v>2030</v>
       </c>
-      <c r="D144" s="45">
+      <c r="E144" s="35">
         <v>2035</v>
       </c>
-      <c r="E144" s="45">
+      <c r="F144" s="35">
         <v>2040</v>
       </c>
-      <c r="F144" s="45">
+      <c r="G144" s="35">
         <v>2045</v>
       </c>
-      <c r="G144" s="45">
+      <c r="H144" s="35">
         <v>2050</v>
       </c>
-      <c r="H144" s="45">
+      <c r="I144" s="35">
         <v>2055</v>
       </c>
-      <c r="I144" s="45">
+      <c r="J144" s="35">
         <v>2060</v>
       </c>
-      <c r="J144" s="45">
+      <c r="K144" s="35">
         <v>2065</v>
       </c>
-      <c r="K144" s="45">
+      <c r="L144" s="35">
         <v>2070</v>
       </c>
-      <c r="L144" s="45">
+      <c r="M144" s="35">
         <v>2075</v>
       </c>
-      <c r="M144" s="45">
+      <c r="N144" s="35">
         <v>2080</v>
       </c>
-      <c r="N144" s="45">
+      <c r="O144" s="35">
         <v>2085</v>
       </c>
-      <c r="O144" s="45">
+      <c r="P144" s="35">
         <v>2090</v>
       </c>
-      <c r="P144" s="45">
+      <c r="Q144" s="35">
         <v>2095</v>
       </c>
-      <c r="Q144" s="45">
+      <c r="R144" s="35">
         <v>2100</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="116" x14ac:dyDescent="0.35">
-      <c r="A145" s="33" t="s">
+    <row r="145" spans="1:18" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B145" s="44">
-        <f>(($B142*B144+$A142)/100)*B83</f>
+      <c r="B145" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C145" s="47">
+        <f>(($B142*C144+$A142)/100)*B83</f>
         <v>11232.769782500007</v>
       </c>
-      <c r="C145" s="44">
-        <f t="shared" ref="C145:Q145" si="9">(($B142*C144+$A142)/100)*C83</f>
+      <c r="D145" s="47">
+        <f>(($B142*D144+$A142)/100)*C83</f>
         <v>11438.18222328</v>
       </c>
-      <c r="D145" s="44">
-        <f t="shared" si="9"/>
+      <c r="E145" s="47">
+        <f>(($B142*E144+$A142)/100)*D83</f>
         <v>11561.455342979998</v>
       </c>
-      <c r="E145" s="44">
-        <f t="shared" si="9"/>
+      <c r="F145" s="47">
+        <f>(($B142*F144+$A142)/100)*E83</f>
         <v>11601.144488280008</v>
       </c>
-      <c r="F145" s="44">
-        <f t="shared" si="9"/>
+      <c r="G145" s="47">
+        <f>(($B142*G144+$A142)/100)*F83</f>
         <v>11555.878831380005</v>
       </c>
-      <c r="G145" s="44">
-        <f t="shared" si="9"/>
+      <c r="H145" s="47">
+        <f>(($B142*H144+$A142)/100)*G83</f>
         <v>11423.608762499996</v>
       </c>
-      <c r="H145" s="44">
-        <f t="shared" si="9"/>
+      <c r="I145" s="47">
+        <f>(($B142*I144+$A142)/100)*H83</f>
         <v>11172.059938899991</v>
       </c>
-      <c r="I145" s="44">
-        <f t="shared" si="9"/>
+      <c r="J145" s="47">
+        <f>(($B142*J144+$A142)/100)*I83</f>
         <v>10849.798171380005</v>
       </c>
-      <c r="J145" s="44">
-        <f t="shared" si="9"/>
+      <c r="K145" s="47">
+        <f>(($B142*K144+$A142)/100)*J83</f>
         <v>10527.866247959999</v>
       </c>
-      <c r="K145" s="44">
-        <f t="shared" si="9"/>
+      <c r="L145" s="47">
+        <f>(($B142*L144+$A142)/100)*K83</f>
         <v>10211.048344719989</v>
       </c>
-      <c r="L145" s="44">
-        <f t="shared" si="9"/>
+      <c r="M145" s="47">
+        <f>(($B142*M144+$A142)/100)*L83</f>
         <v>9871.7309883000053</v>
       </c>
-      <c r="M145" s="44">
-        <f t="shared" si="9"/>
+      <c r="N145" s="47">
+        <f>(($B142*N144+$A142)/100)*M83</f>
         <v>9465.8934329200001</v>
       </c>
-      <c r="N145" s="44">
-        <f t="shared" si="9"/>
+      <c r="O145" s="47">
+        <f>(($B142*O144+$A142)/100)*N83</f>
         <v>9025.2317390799908</v>
       </c>
-      <c r="O145" s="44">
-        <f t="shared" si="9"/>
+      <c r="P145" s="47">
+        <f>(($B142*P144+$A142)/100)*O83</f>
         <v>8586.6460133400069</v>
       </c>
-      <c r="P145" s="44">
-        <f t="shared" si="9"/>
+      <c r="Q145" s="47">
+        <f>(($B142*Q144+$A142)/100)*P83</f>
         <v>8154.376048420002</v>
       </c>
-      <c r="Q145" s="44">
-        <f t="shared" si="9"/>
+      <c r="R145" s="47">
+        <f>(($B142*R144+$A142)/100)*Q83</f>
         <v>7726.0072344999935</v>
       </c>
     </row>
+    <row r="146" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A146" s="37"/>
+      <c r="B146" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C146" s="34">
+        <f>$S137*B83</f>
+        <v>11626.37088</v>
+      </c>
+      <c r="D146" s="34">
+        <f t="shared" ref="D146:R146" si="10">$S137*C83</f>
+        <v>12156.155135999999</v>
+      </c>
+      <c r="E146" s="34">
+        <f t="shared" si="10"/>
+        <v>12625.409088000002</v>
+      </c>
+      <c r="F146" s="34">
+        <f t="shared" si="10"/>
+        <v>13027.370112000001</v>
+      </c>
+      <c r="G146" s="34">
+        <f t="shared" si="10"/>
+        <v>13354.572864000002</v>
+      </c>
+      <c r="H146" s="34">
+        <f t="shared" si="10"/>
+        <v>13597.848</v>
+      </c>
+      <c r="I146" s="34">
+        <f t="shared" si="10"/>
+        <v>13709.80128</v>
+      </c>
+      <c r="J146" s="34">
+        <f t="shared" si="10"/>
+        <v>13739.356608000002</v>
+      </c>
+      <c r="K146" s="34">
+        <f t="shared" si="10"/>
+        <v>13771.292544000002</v>
+      </c>
+      <c r="L146" s="34">
+        <f t="shared" si="10"/>
+        <v>13812.324095999998</v>
+      </c>
+      <c r="M146" s="34">
+        <f t="shared" si="10"/>
+        <v>13824.743615999998</v>
+      </c>
+      <c r="N146" s="34">
+        <f t="shared" si="10"/>
+        <v>13741.505664</v>
+      </c>
+      <c r="O146" s="34">
+        <f t="shared" si="10"/>
+        <v>13599.470207999999</v>
+      </c>
+      <c r="P146" s="34">
+        <f t="shared" si="10"/>
+        <v>13449.470016000001</v>
+      </c>
+      <c r="Q146" s="34">
+        <f t="shared" si="10"/>
+        <v>13297.436736000001</v>
+      </c>
+      <c r="R146" s="34">
+        <f t="shared" si="10"/>
+        <v>13139.002559999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A38:P38"/>
     <mergeCell ref="I90:J90"/>
     <mergeCell ref="A133:H133"/>
     <mergeCell ref="A58:P58"/>
     <mergeCell ref="A79:Q79"/>
     <mergeCell ref="A86:H86"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A38:P38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cleanup Excel documents and organize loading and saving of parameters from Excel documents in mat files by topic. Get rid of reliance on calibratedParams.mat file: either hardcode values or set from Excel docs.
</commit_message>
<xml_diff>
--- a/Config/Population_validation_targets.xlsx
+++ b/Config/Population_validation_targets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
   <si>
     <t>1950-1955</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Population in South Africa (thousands)</t>
   </si>
   <si>
-    <t>Statistical Release P0301 Community Survey 2016 Table 2.1: Censuss 2011 and Community Survey 2016.</t>
-  </si>
-  <si>
     <t>Total Males and Females to 69</t>
   </si>
   <si>
@@ -227,16 +224,10 @@
     <t>SOUTH AFRICA COMPARISON</t>
   </si>
   <si>
-    <t>Statistical Release P0302 2019 Mid-year population estimates Table 6 and Table 11.</t>
-  </si>
-  <si>
     <t>Statistics South Africa. Primary tables Census '96 and 2001 compared. KwaZulu-Natal Table 4.1 and 4.3. South Africa Table 4.1.</t>
   </si>
   <si>
     <t>Population in KZN (and South Africa comparison)</t>
-  </si>
-  <si>
-    <t>Statistical Release P0302 2019 Mid-year population estimates Table 5.3</t>
   </si>
   <si>
     <t>Percent</t>
@@ -279,6 +270,15 @@
   </si>
   <si>
     <t>Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing in the past. Assume male and female populations by age follow exponential distributions. Highlighted values transferred to Population_data Excel doc.</t>
+  </si>
+  <si>
+    <t>Statistics South Africa Statistical Release P0301 Community Survey 2016 Table 2.1: Censuss 2011 and Community Survey 2016.</t>
+  </si>
+  <si>
+    <t>Statistics South Africa Statistical Release P0302 2019 Mid-year population estimates Table 6 and Table 11.</t>
+  </si>
+  <si>
+    <t>Statistics South Africa Statistical Release P0302 2019 Mid-year population estimates Table 5.3</t>
   </si>
 </sst>
 </file>
@@ -501,6 +501,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -531,27 +552,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2582,7 +2582,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2621,7 +2621,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$191:$K$191</c:f>
+              <c:f>Demographics!$B$192:$K$192</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2699,7 +2699,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$M$153</c:f>
+              <c:f>Demographics!$M$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -2711,7 +2711,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$M$191</c:f>
+              <c:f>Demographics!$M$192</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3504,7 +3504,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$154</c:f>
+              <c:f>Demographics!$A$155</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3553,7 +3553,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3592,7 +3592,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$154:$K$154</c:f>
+              <c:f>Demographics!$B$155:$K$155</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3641,7 +3641,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$155</c:f>
+              <c:f>Demographics!$A$156</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3690,7 +3690,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3729,7 +3729,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$155:$K$155</c:f>
+              <c:f>Demographics!$B$156:$K$156</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3778,7 +3778,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$156</c:f>
+              <c:f>Demographics!$A$157</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3827,7 +3827,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3866,7 +3866,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$156:$K$156</c:f>
+              <c:f>Demographics!$B$157:$K$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3915,7 +3915,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$157</c:f>
+              <c:f>Demographics!$A$158</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3964,7 +3964,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4003,7 +4003,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$157:$K$157</c:f>
+              <c:f>Demographics!$B$158:$K$158</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4052,7 +4052,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$158</c:f>
+              <c:f>Demographics!$A$159</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4101,7 +4101,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4140,7 +4140,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$158:$K$158</c:f>
+              <c:f>Demographics!$B$159:$K$159</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4189,7 +4189,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$159</c:f>
+              <c:f>Demographics!$A$160</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4238,7 +4238,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4277,7 +4277,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$159:$K$159</c:f>
+              <c:f>Demographics!$B$160:$K$160</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4326,7 +4326,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$160</c:f>
+              <c:f>Demographics!$A$161</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4383,7 +4383,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4422,7 +4422,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$160:$K$160</c:f>
+              <c:f>Demographics!$B$161:$K$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4471,7 +4471,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$161</c:f>
+              <c:f>Demographics!$A$162</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4528,7 +4528,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4567,7 +4567,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$161:$K$161</c:f>
+              <c:f>Demographics!$B$162:$K$162</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4616,7 +4616,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$162</c:f>
+              <c:f>Demographics!$A$163</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4673,7 +4673,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4712,7 +4712,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$162:$K$162</c:f>
+              <c:f>Demographics!$B$163:$K$163</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4761,7 +4761,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$163</c:f>
+              <c:f>Demographics!$A$164</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4818,7 +4818,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4857,7 +4857,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$163:$K$163</c:f>
+              <c:f>Demographics!$B$164:$K$164</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4906,7 +4906,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$164</c:f>
+              <c:f>Demographics!$A$165</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4963,7 +4963,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5002,7 +5002,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$164:$K$164</c:f>
+              <c:f>Demographics!$B$165:$K$165</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5051,7 +5051,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$165</c:f>
+              <c:f>Demographics!$A$166</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5108,7 +5108,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5147,7 +5147,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$165:$K$165</c:f>
+              <c:f>Demographics!$B$166:$K$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5196,7 +5196,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$166</c:f>
+              <c:f>Demographics!$A$167</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5257,7 +5257,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5296,7 +5296,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$166:$K$166</c:f>
+              <c:f>Demographics!$B$167:$K$167</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5345,7 +5345,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$167</c:f>
+              <c:f>Demographics!$A$168</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5406,7 +5406,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5445,7 +5445,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$167:$K$167</c:f>
+              <c:f>Demographics!$B$168:$K$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5494,7 +5494,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$168</c:f>
+              <c:f>Demographics!$A$169</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5555,7 +5555,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5594,7 +5594,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$168:$K$168</c:f>
+              <c:f>Demographics!$B$169:$K$169</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5643,7 +5643,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$169</c:f>
+              <c:f>Demographics!$A$170</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5704,7 +5704,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$153:$K$153</c:f>
+              <c:f>Demographics!$B$154:$K$154</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5743,7 +5743,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$169:$K$169</c:f>
+              <c:f>Demographics!$B$170:$K$170</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6080,7 +6080,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$174</c:f>
+              <c:f>Demographics!$A$175</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6129,7 +6129,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6168,7 +6168,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$174:$K$174</c:f>
+              <c:f>Demographics!$B$175:$K$175</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6217,7 +6217,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$175</c:f>
+              <c:f>Demographics!$A$176</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6266,7 +6266,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6305,7 +6305,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$175:$K$175</c:f>
+              <c:f>Demographics!$B$176:$K$176</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6354,7 +6354,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$176</c:f>
+              <c:f>Demographics!$A$177</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6403,7 +6403,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6442,7 +6442,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$176:$K$176</c:f>
+              <c:f>Demographics!$B$177:$K$177</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6491,7 +6491,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$177</c:f>
+              <c:f>Demographics!$A$178</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6540,7 +6540,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6579,7 +6579,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$177:$K$177</c:f>
+              <c:f>Demographics!$B$178:$K$178</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6628,7 +6628,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$178</c:f>
+              <c:f>Demographics!$A$179</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6677,7 +6677,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6716,7 +6716,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$178:$K$178</c:f>
+              <c:f>Demographics!$B$179:$K$179</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6765,7 +6765,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$179</c:f>
+              <c:f>Demographics!$A$180</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6814,7 +6814,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6853,7 +6853,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$179:$K$179</c:f>
+              <c:f>Demographics!$B$180:$K$180</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6902,7 +6902,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$180</c:f>
+              <c:f>Demographics!$A$181</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6959,7 +6959,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6998,7 +6998,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$180:$K$180</c:f>
+              <c:f>Demographics!$B$181:$K$181</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7047,7 +7047,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$181</c:f>
+              <c:f>Demographics!$A$182</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7104,7 +7104,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7143,7 +7143,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$181:$K$181</c:f>
+              <c:f>Demographics!$B$182:$K$182</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7192,7 +7192,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$182</c:f>
+              <c:f>Demographics!$A$183</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7249,7 +7249,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7288,7 +7288,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$182:$K$182</c:f>
+              <c:f>Demographics!$B$183:$K$183</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7337,7 +7337,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$183</c:f>
+              <c:f>Demographics!$A$184</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7394,7 +7394,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7433,7 +7433,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$183:$K$183</c:f>
+              <c:f>Demographics!$B$184:$K$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7482,7 +7482,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$184</c:f>
+              <c:f>Demographics!$A$185</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7539,7 +7539,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7578,7 +7578,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$184:$K$184</c:f>
+              <c:f>Demographics!$B$185:$K$185</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7627,7 +7627,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$185</c:f>
+              <c:f>Demographics!$A$186</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7684,7 +7684,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7723,7 +7723,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$185:$K$185</c:f>
+              <c:f>Demographics!$B$186:$K$186</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7772,7 +7772,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$186</c:f>
+              <c:f>Demographics!$A$187</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7833,7 +7833,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7872,7 +7872,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$186:$K$186</c:f>
+              <c:f>Demographics!$B$187:$K$187</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -7921,7 +7921,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$187</c:f>
+              <c:f>Demographics!$A$188</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7982,7 +7982,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8021,7 +8021,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$187:$K$187</c:f>
+              <c:f>Demographics!$B$188:$K$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8070,7 +8070,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$188</c:f>
+              <c:f>Demographics!$A$189</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8131,7 +8131,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8170,7 +8170,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$188:$K$188</c:f>
+              <c:f>Demographics!$B$189:$K$189</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8219,7 +8219,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Demographics!$A$189</c:f>
+              <c:f>Demographics!$A$190</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8280,7 +8280,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Demographics!$B$173:$K$173</c:f>
+              <c:f>Demographics!$B$174:$K$174</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -8319,7 +8319,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Demographics!$B$189:$K$189</c:f>
+              <c:f>Demographics!$B$190:$K$190</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -11451,13 +11451,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>334737</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>10079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>184454</xdr:colOff>
-      <xdr:row>176</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>104240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11481,13 +11481,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>147204</xdr:colOff>
-      <xdr:row>175</xdr:row>
+      <xdr:row>176</xdr:row>
       <xdr:rowOff>68696</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>46181</xdr:colOff>
-      <xdr:row>202</xdr:row>
+      <xdr:row>203</xdr:row>
       <xdr:rowOff>80818</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11773,10 +11773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA191"/>
+  <dimension ref="A1:AA192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC169" sqref="AC169"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F198" sqref="F198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11791,16 +11791,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -11822,16 +11822,16 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -12500,16 +12500,16 @@
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -12531,16 +12531,16 @@
       <c r="AA36" s="1"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -12562,24 +12562,24 @@
       <c r="AA37" s="1"/>
     </row>
     <row r="38" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="43"/>
-      <c r="O38" s="43"/>
-      <c r="P38" s="44"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="61"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
@@ -13498,24 +13498,24 @@
       <c r="A57" s="10"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A58" s="45" t="s">
+      <c r="A58" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="46"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="46"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="46"/>
-      <c r="N58" s="46"/>
-      <c r="O58" s="46"/>
-      <c r="P58" s="47"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="63"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="63"/>
+      <c r="O58" s="63"/>
+      <c r="P58" s="64"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="7"/>
@@ -14496,25 +14496,25 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A79" s="48" t="s">
+      <c r="A79" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="48"/>
-      <c r="C79" s="48"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="48"/>
-      <c r="I79" s="48"/>
-      <c r="J79" s="48"/>
-      <c r="K79" s="48"/>
-      <c r="L79" s="48"/>
-      <c r="M79" s="48"/>
-      <c r="N79" s="48"/>
-      <c r="O79" s="48"/>
-      <c r="P79" s="48"/>
-      <c r="Q79" s="48"/>
+      <c r="B79" s="65"/>
+      <c r="C79" s="65"/>
+      <c r="D79" s="65"/>
+      <c r="E79" s="65"/>
+      <c r="F79" s="65"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="65"/>
+      <c r="J79" s="65"/>
+      <c r="K79" s="65"/>
+      <c r="L79" s="65"/>
+      <c r="M79" s="65"/>
+      <c r="N79" s="65"/>
+      <c r="O79" s="65"/>
+      <c r="P79" s="65"/>
+      <c r="Q79" s="65"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="4"/>
@@ -14745,16 +14745,16 @@
       <c r="A85" s="19"/>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A86" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40"/>
-      <c r="F86" s="40"/>
-      <c r="G86" s="40"/>
-      <c r="H86" s="40"/>
+      <c r="A86" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" s="57"/>
+      <c r="C86" s="57"/>
+      <c r="D86" s="57"/>
+      <c r="E86" s="57"/>
+      <c r="F86" s="57"/>
+      <c r="G86" s="57"/>
+      <c r="H86" s="57"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -14777,7 +14777,7 @@
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
@@ -14808,7 +14808,7 @@
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
@@ -14839,7 +14839,7 @@
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A89" s="23" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
@@ -14887,12 +14887,12 @@
       </c>
       <c r="G90" s="21"/>
       <c r="H90" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="I90" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="I90" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="J90" s="39"/>
+      <c r="J90" s="56"/>
       <c r="K90" s="21"/>
       <c r="L90" s="21"/>
       <c r="M90" s="21"/>
@@ -15073,7 +15073,7 @@
       </c>
       <c r="G96" s="19"/>
       <c r="H96" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I96" s="4">
         <f>40583573-178902-137284</f>
@@ -15109,7 +15109,7 @@
       </c>
       <c r="G97" s="19"/>
       <c r="H97" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I97" s="4">
         <f>I96/1000</f>
@@ -15980,7 +15980,7 @@
     </row>
     <row r="129" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A129" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B129">
         <f>B108+B128</f>
@@ -16005,7 +16005,7 @@
     </row>
     <row r="130" spans="1:27" ht="58" x14ac:dyDescent="0.35">
       <c r="A130" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B130" s="1">
         <f>B129/1000</f>
@@ -16029,16 +16029,16 @@
       </c>
     </row>
     <row r="133" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A133" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="B133" s="58"/>
-      <c r="C133" s="58"/>
-      <c r="D133" s="58"/>
-      <c r="E133" s="58"/>
-      <c r="F133" s="58"/>
-      <c r="G133" s="58"/>
-      <c r="H133" s="58"/>
+      <c r="A133" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B133" s="47"/>
+      <c r="C133" s="47"/>
+      <c r="D133" s="47"/>
+      <c r="E133" s="47"/>
+      <c r="F133" s="47"/>
+      <c r="G133" s="47"/>
+      <c r="H133" s="47"/>
       <c r="I133" s="1"/>
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
@@ -16061,7 +16061,7 @@
     </row>
     <row r="134" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A134" s="23" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B134" s="22"/>
       <c r="C134" s="22"/>
@@ -16166,7 +16166,7 @@
     </row>
     <row r="136" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A136" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B136" s="29">
         <v>20.8</v>
@@ -16225,7 +16225,7 @@
     </row>
     <row r="137" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A137" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B137" s="4">
         <f>B136/100</f>
@@ -16302,7 +16302,7 @@
     </row>
     <row r="138" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A138" s="33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E138">
         <f>E137*M77</f>
@@ -16326,10 +16326,10 @@
     </row>
     <row r="141" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A141" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="142" spans="1:27" x14ac:dyDescent="0.35">
@@ -16394,11 +16394,11 @@
       </c>
     </row>
     <row r="145" spans="1:27" ht="76" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="39" t="s">
-        <v>76</v>
+      <c r="A145" s="56" t="s">
+        <v>73</v>
       </c>
       <c r="B145" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C145" s="37">
         <f t="shared" ref="C145:R145" si="10">(($B142*C144+$A142)/100)*B83</f>
@@ -16466,9 +16466,9 @@
       </c>
     </row>
     <row r="146" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A146" s="39"/>
+      <c r="A146" s="56"/>
       <c r="B146" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C146" s="34">
         <f>$S137*B83</f>
@@ -16536,8 +16536,8 @@
       </c>
     </row>
     <row r="149" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A149" s="64" t="s">
-        <v>83</v>
+      <c r="A149" s="53" t="s">
+        <v>80</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -16567,16 +16567,16 @@
       <c r="AA149" s="1"/>
     </row>
     <row r="150" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A150" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-      <c r="G150" s="1"/>
-      <c r="H150" s="1"/>
+      <c r="A150" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B150" s="58"/>
+      <c r="C150" s="58"/>
+      <c r="D150" s="58"/>
+      <c r="E150" s="58"/>
+      <c r="F150" s="58"/>
+      <c r="G150" s="58"/>
+      <c r="H150" s="58"/>
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
@@ -16597,2046 +16597,2108 @@
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
     </row>
+    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A151" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+      <c r="T151" s="1"/>
+      <c r="U151" s="1"/>
+      <c r="V151" s="1"/>
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+      <c r="Y151" s="1"/>
+      <c r="Z151" s="1"/>
+      <c r="AA151" s="1"/>
+    </row>
     <row r="152" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A152" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B152" s="51"/>
-      <c r="C152" s="51"/>
-      <c r="D152" s="51"/>
-      <c r="E152" s="51"/>
-      <c r="F152" s="51"/>
-      <c r="G152" s="51"/>
-      <c r="H152" s="51"/>
-      <c r="I152" s="51"/>
-      <c r="J152" s="51"/>
-      <c r="K152" s="51"/>
-      <c r="L152" s="52"/>
+      <c r="A152" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="N152" s="1"/>
+      <c r="O152" s="1"/>
+      <c r="P152" s="1"/>
+      <c r="Q152" s="1"/>
+      <c r="R152" s="1"/>
+      <c r="S152" s="1"/>
+      <c r="T152" s="1"/>
+      <c r="U152" s="1"/>
+      <c r="V152" s="1"/>
+      <c r="W152" s="1"/>
+      <c r="X152" s="1"/>
+      <c r="Y152" s="1"/>
+      <c r="Z152" s="1"/>
+      <c r="AA152" s="1"/>
     </row>
     <row r="153" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A153" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B153" s="7">
-        <v>1950</v>
-      </c>
-      <c r="C153" s="7">
-        <v>1955</v>
-      </c>
-      <c r="D153" s="7">
-        <v>1960</v>
-      </c>
-      <c r="E153" s="7">
-        <v>1965</v>
-      </c>
-      <c r="F153" s="7">
-        <v>1970</v>
-      </c>
-      <c r="G153" s="7">
-        <v>1975</v>
-      </c>
-      <c r="H153" s="7">
-        <v>1980</v>
-      </c>
-      <c r="I153" s="7">
-        <v>1985</v>
-      </c>
-      <c r="J153" s="7">
-        <v>1990</v>
-      </c>
-      <c r="K153" s="7">
-        <v>1995</v>
-      </c>
-      <c r="M153" s="27">
-        <v>1910</v>
-      </c>
-      <c r="O153" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="P153" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="A153" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B153" s="55"/>
+      <c r="C153" s="55"/>
+      <c r="D153" s="55"/>
+      <c r="E153" s="55"/>
+      <c r="F153" s="55"/>
+      <c r="G153" s="55"/>
+      <c r="H153" s="55"/>
+      <c r="I153" s="55"/>
+      <c r="J153" s="55"/>
+      <c r="K153" s="55"/>
+      <c r="L153" s="41"/>
     </row>
     <row r="154" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A154" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B154" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B40</f>
-        <v>261.71339999999998</v>
-      </c>
-      <c r="C154" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C40</f>
-        <v>317.33477999999991</v>
-      </c>
-      <c r="D154" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D40</f>
-        <v>353.00481999999977</v>
-      </c>
-      <c r="E154" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E40</f>
-        <v>389.24084000000005</v>
-      </c>
-      <c r="F154" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F40</f>
-        <v>425.19593999999989</v>
-      </c>
-      <c r="G154" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G40</f>
-        <v>471.5423999999997</v>
-      </c>
-      <c r="H154" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H40</f>
-        <v>512.40722000000017</v>
-      </c>
-      <c r="I154" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I40</f>
-        <v>582.74777999999992</v>
-      </c>
-      <c r="J154" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J40</f>
-        <v>601.97871999999973</v>
-      </c>
-      <c r="K154" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K40</f>
-        <v>554.80044000000021</v>
-      </c>
-      <c r="M154" s="65">
-        <f>O154*EXP($M$153*P154)</f>
-        <v>116.45919703766468</v>
-      </c>
-      <c r="O154" s="49">
-        <v>2.0000000000000001E-13</v>
-      </c>
-      <c r="P154" s="50">
-        <v>1.78E-2</v>
+      <c r="A154" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B154" s="7">
+        <v>1950</v>
+      </c>
+      <c r="C154" s="7">
+        <v>1955</v>
+      </c>
+      <c r="D154" s="7">
+        <v>1960</v>
+      </c>
+      <c r="E154" s="7">
+        <v>1965</v>
+      </c>
+      <c r="F154" s="7">
+        <v>1970</v>
+      </c>
+      <c r="G154" s="7">
+        <v>1975</v>
+      </c>
+      <c r="H154" s="7">
+        <v>1980</v>
+      </c>
+      <c r="I154" s="7">
+        <v>1985</v>
+      </c>
+      <c r="J154" s="7">
+        <v>1990</v>
+      </c>
+      <c r="K154" s="7">
+        <v>1995</v>
+      </c>
+      <c r="M154" s="27">
+        <v>1910</v>
+      </c>
+      <c r="O154" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P154" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="155" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A155" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B155" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B41</f>
-        <v>220.41739999999999</v>
+        <f>(($B$142*B$154+$A$142)/100)*B40</f>
+        <v>261.71339999999998</v>
       </c>
       <c r="C155" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C41</f>
-        <v>234.26549999999995</v>
+        <f>(($B$142*C$154+$A$142)/100)*C40</f>
+        <v>317.33477999999991</v>
       </c>
       <c r="D155" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D41</f>
-        <v>288.91245999999978</v>
+        <f>(($B$142*D$154+$A$142)/100)*D40</f>
+        <v>353.00481999999977</v>
       </c>
       <c r="E155" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E41</f>
-        <v>324.20498000000003</v>
+        <f>(($B$142*E$154+$A$142)/100)*E40</f>
+        <v>389.24084000000005</v>
       </c>
       <c r="F155" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F41</f>
-        <v>360.97487999999993</v>
+        <f>(($B$142*F$154+$A$142)/100)*F40</f>
+        <v>425.19593999999989</v>
       </c>
       <c r="G155" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G41</f>
-        <v>399.26729999999975</v>
+        <f>(($B$142*G$154+$A$142)/100)*G40</f>
+        <v>471.5423999999997</v>
       </c>
       <c r="H155" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H41</f>
-        <v>447.35418000000016</v>
+        <f>(($B$142*H$154+$A$142)/100)*H40</f>
+        <v>512.40722000000017</v>
       </c>
       <c r="I155" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I41</f>
-        <v>490.59335999999996</v>
+        <f>(($B$142*I$154+$A$142)/100)*I40</f>
+        <v>582.74777999999992</v>
       </c>
       <c r="J155" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J41</f>
-        <v>558.76085999999975</v>
+        <f>(($B$142*J$154+$A$142)/100)*J40</f>
+        <v>601.97871999999973</v>
       </c>
       <c r="K155" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K41</f>
-        <v>579.25800000000015</v>
-      </c>
-      <c r="M155" s="65">
-        <f t="shared" ref="M155:M169" si="12">O155*EXP($M$153*P155)</f>
-        <v>76.187743222862409</v>
-      </c>
-      <c r="O155" s="49">
-        <v>2.0000000000000001E-17</v>
-      </c>
-      <c r="P155" s="50">
-        <v>2.24E-2</v>
+        <f>(($B$142*K$154+$A$142)/100)*K40</f>
+        <v>554.80044000000021</v>
+      </c>
+      <c r="M155" s="54">
+        <f>O155*EXP($M$154*P155)</f>
+        <v>116.45919703766468</v>
+      </c>
+      <c r="O155" s="39">
+        <v>2.0000000000000001E-13</v>
+      </c>
+      <c r="P155" s="40">
+        <v>1.78E-2</v>
       </c>
     </row>
     <row r="156" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A156" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B156" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B42</f>
-        <v>191.76830000000001</v>
+        <f>(($B$142*B$154+$A$142)/100)*B41</f>
+        <v>220.41739999999999</v>
       </c>
       <c r="C156" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C42</f>
-        <v>209.19275999999994</v>
+        <f>(($B$142*C$154+$A$142)/100)*C41</f>
+        <v>234.26549999999995</v>
       </c>
       <c r="D156" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D42</f>
-        <v>223.32957999999985</v>
+        <f>(($B$142*D$154+$A$142)/100)*D41</f>
+        <v>288.91245999999978</v>
       </c>
       <c r="E156" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E42</f>
-        <v>276.21972000000005</v>
+        <f>(($B$142*E$154+$A$142)/100)*E41</f>
+        <v>324.20498000000003</v>
       </c>
       <c r="F156" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F42</f>
-        <v>311.31695999999994</v>
+        <f>(($B$142*F$154+$A$142)/100)*F41</f>
+        <v>360.97487999999993</v>
       </c>
       <c r="G156" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G42</f>
-        <v>348.04319999999979</v>
+        <f>(($B$142*G$154+$A$142)/100)*G41</f>
+        <v>399.26729999999975</v>
       </c>
       <c r="H156" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H42</f>
-        <v>385.27892000000014</v>
+        <f>(($B$142*H$154+$A$142)/100)*H41</f>
+        <v>447.35418000000016</v>
       </c>
       <c r="I156" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I42</f>
-        <v>432.52037999999993</v>
+        <f>(($B$142*I$154+$A$142)/100)*I41</f>
+        <v>490.59335999999996</v>
       </c>
       <c r="J156" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J42</f>
-        <v>473.86079999999976</v>
+        <f>(($B$142*J$154+$A$142)/100)*J41</f>
+        <v>558.76085999999975</v>
       </c>
       <c r="K156" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K42</f>
-        <v>541.28442000000018</v>
-      </c>
-      <c r="M156" s="65">
-        <f t="shared" si="12"/>
-        <v>75.385542052984889</v>
-      </c>
-      <c r="O156" s="49">
-        <v>2.0000000000000001E-18</v>
-      </c>
-      <c r="P156" s="50">
-        <v>2.3599999999999999E-2</v>
+        <f>(($B$142*K$154+$A$142)/100)*K41</f>
+        <v>579.25800000000015</v>
+      </c>
+      <c r="M156" s="54">
+        <f t="shared" ref="M156:M170" si="12">O156*EXP($M$154*P156)</f>
+        <v>76.187743222862409</v>
+      </c>
+      <c r="O156" s="39">
+        <v>2.0000000000000001E-17</v>
+      </c>
+      <c r="P156" s="40">
+        <v>2.24E-2</v>
       </c>
     </row>
     <row r="157" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A157" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B157" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B43</f>
-        <v>177.0566</v>
+        <f>(($B$142*B$154+$A$142)/100)*B42</f>
+        <v>191.76830000000001</v>
       </c>
       <c r="C157" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C43</f>
-        <v>183.36023999999995</v>
+        <f>(($B$142*C$154+$A$142)/100)*C42</f>
+        <v>209.19275999999994</v>
       </c>
       <c r="D157" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D43</f>
-        <v>200.47493999999986</v>
+        <f>(($B$142*D$154+$A$142)/100)*D42</f>
+        <v>223.32957999999985</v>
       </c>
       <c r="E157" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E43</f>
-        <v>215.56830000000005</v>
+        <f>(($B$142*E$154+$A$142)/100)*E42</f>
+        <v>276.21972000000005</v>
       </c>
       <c r="F157" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F43</f>
-        <v>267.38879999999995</v>
+        <f>(($B$142*F$154+$A$142)/100)*F42</f>
+        <v>311.31695999999994</v>
       </c>
       <c r="G157" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G43</f>
-        <v>301.49709999999982</v>
+        <f>(($B$142*G$154+$A$142)/100)*G42</f>
+        <v>348.04319999999979</v>
       </c>
       <c r="H157" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H43</f>
-        <v>336.71820000000008</v>
+        <f>(($B$142*H$154+$A$142)/100)*H42</f>
+        <v>385.27892000000014</v>
       </c>
       <c r="I157" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I43</f>
-        <v>373.77473999999995</v>
+        <f>(($B$142*I$154+$A$142)/100)*I42</f>
+        <v>432.52037999999993</v>
       </c>
       <c r="J157" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J43</f>
-        <v>417.48013999999978</v>
+        <f>(($B$142*J$154+$A$142)/100)*J42</f>
+        <v>473.86079999999976</v>
       </c>
       <c r="K157" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K43</f>
-        <v>461.47554000000014</v>
-      </c>
-      <c r="M157" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K42</f>
+        <v>541.28442000000018</v>
+      </c>
+      <c r="M157" s="54">
         <f t="shared" si="12"/>
-        <v>71.896515135187158</v>
-      </c>
-      <c r="O157" s="49">
-        <v>5.9999999999999997E-18</v>
-      </c>
-      <c r="P157" s="50">
-        <v>2.3E-2</v>
+        <v>75.385542052984889</v>
+      </c>
+      <c r="O157" s="39">
+        <v>2.0000000000000001E-18</v>
+      </c>
+      <c r="P157" s="40">
+        <v>2.3599999999999999E-2</v>
       </c>
     </row>
     <row r="158" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A158" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B158" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B44</f>
-        <v>160.02199999999999</v>
+        <f>(($B$142*B$154+$A$142)/100)*B43</f>
+        <v>177.0566</v>
       </c>
       <c r="C158" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C44</f>
-        <v>167.65811999999994</v>
+        <f>(($B$142*C$154+$A$142)/100)*C43</f>
+        <v>183.36023999999995</v>
       </c>
       <c r="D158" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D44</f>
-        <v>174.39083999999988</v>
+        <f>(($B$142*D$154+$A$142)/100)*D43</f>
+        <v>200.47493999999986</v>
       </c>
       <c r="E158" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E44</f>
-        <v>193.64610000000005</v>
+        <f>(($B$142*E$154+$A$142)/100)*E43</f>
+        <v>215.56830000000005</v>
       </c>
       <c r="F158" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F44</f>
-        <v>210.09119999999996</v>
+        <f>(($B$142*F$154+$A$142)/100)*F43</f>
+        <v>267.38879999999995</v>
       </c>
       <c r="G158" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G44</f>
-        <v>259.62899999999985</v>
+        <f>(($B$142*G$154+$A$142)/100)*G43</f>
+        <v>301.49709999999982</v>
       </c>
       <c r="H158" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H44</f>
-        <v>290.44808000000006</v>
+        <f>(($B$142*H$154+$A$142)/100)*H43</f>
+        <v>336.71820000000008</v>
       </c>
       <c r="I158" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I44</f>
-        <v>326.24009999999998</v>
+        <f>(($B$142*I$154+$A$142)/100)*I43</f>
+        <v>373.77473999999995</v>
       </c>
       <c r="J158" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J44</f>
-        <v>357.37001999999978</v>
+        <f>(($B$142*J$154+$A$142)/100)*J43</f>
+        <v>417.48013999999978</v>
       </c>
       <c r="K158" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K44</f>
-        <v>409.34232000000014</v>
-      </c>
-      <c r="M158" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K43</f>
+        <v>461.47554000000014</v>
+      </c>
+      <c r="M158" s="54">
         <f t="shared" si="12"/>
-        <v>51.997757864486189</v>
-      </c>
-      <c r="O158" s="49">
-        <v>2.0000000000000001E-17</v>
-      </c>
-      <c r="P158" s="50">
-        <v>2.2200000000000001E-2</v>
+        <v>71.896515135187158</v>
+      </c>
+      <c r="O158" s="39">
+        <v>5.9999999999999997E-18</v>
+      </c>
+      <c r="P158" s="40">
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="159" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A159" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B159" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B45</f>
-        <v>139.89019999999999</v>
+        <f>(($B$142*B$154+$A$142)/100)*B44</f>
+        <v>160.02199999999999</v>
       </c>
       <c r="C159" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C45</f>
-        <v>150.18317999999996</v>
+        <f>(($B$142*C$154+$A$142)/100)*C44</f>
+        <v>167.65811999999994</v>
       </c>
       <c r="D159" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D45</f>
-        <v>158.24353999999988</v>
+        <f>(($B$142*D$154+$A$142)/100)*D44</f>
+        <v>174.39083999999988</v>
       </c>
       <c r="E159" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E45</f>
-        <v>167.58304000000004</v>
+        <f>(($B$142*E$154+$A$142)/100)*E44</f>
+        <v>193.64610000000005</v>
       </c>
       <c r="F159" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F45</f>
-        <v>189.32081999999997</v>
+        <f>(($B$142*F$154+$A$142)/100)*F44</f>
+        <v>210.09119999999996</v>
       </c>
       <c r="G159" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G45</f>
-        <v>205.59809999999987</v>
+        <f>(($B$142*G$154+$A$142)/100)*G44</f>
+        <v>259.62899999999985</v>
       </c>
       <c r="H159" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H45</f>
-        <v>249.44634000000008</v>
+        <f>(($B$142*H$154+$A$142)/100)*H44</f>
+        <v>290.44808000000006</v>
       </c>
       <c r="I159" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I45</f>
-        <v>282.06875999999994</v>
+        <f>(($B$142*I$154+$A$142)/100)*I44</f>
+        <v>326.24009999999998</v>
       </c>
       <c r="J159" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J45</f>
-        <v>309.98393999999985</v>
+        <f>(($B$142*J$154+$A$142)/100)*J44</f>
+        <v>357.37001999999978</v>
       </c>
       <c r="K159" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K45</f>
-        <v>353.1328400000001</v>
-      </c>
-      <c r="M159" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K44</f>
+        <v>409.34232000000014</v>
+      </c>
+      <c r="M159" s="54">
         <f t="shared" si="12"/>
-        <v>46.60176948050119</v>
-      </c>
-      <c r="O159" s="49">
-        <v>9.9999999999999998E-17</v>
-      </c>
-      <c r="P159" s="50">
-        <v>2.1299999999999999E-2</v>
+        <v>51.997757864486189</v>
+      </c>
+      <c r="O159" s="39">
+        <v>2.0000000000000001E-17</v>
+      </c>
+      <c r="P159" s="40">
+        <v>2.2200000000000001E-2</v>
       </c>
     </row>
     <row r="160" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A160" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B160" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B46</f>
-        <v>126.98519999999999</v>
+        <f>(($B$142*B$154+$A$142)/100)*B45</f>
+        <v>139.89019999999999</v>
       </c>
       <c r="C160" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C46</f>
-        <v>130.68215999999995</v>
+        <f>(($B$142*C$154+$A$142)/100)*C45</f>
+        <v>150.18317999999996</v>
       </c>
       <c r="D160" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D46</f>
-        <v>141.1025599999999</v>
+        <f>(($B$142*D$154+$A$142)/100)*D45</f>
+        <v>158.24353999999988</v>
       </c>
       <c r="E160" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E46</f>
-        <v>151.01960000000003</v>
+        <f>(($B$142*E$154+$A$142)/100)*E45</f>
+        <v>167.58304000000004</v>
       </c>
       <c r="F160" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F46</f>
-        <v>163.53689999999997</v>
+        <f>(($B$142*F$154+$A$142)/100)*F45</f>
+        <v>189.32081999999997</v>
       </c>
       <c r="G160" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G46</f>
-        <v>185.48269999999988</v>
+        <f>(($B$142*G$154+$A$142)/100)*G45</f>
+        <v>205.59809999999987</v>
       </c>
       <c r="H160" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H46</f>
-        <v>197.22066000000007</v>
+        <f>(($B$142*H$154+$A$142)/100)*H45</f>
+        <v>249.44634000000008</v>
       </c>
       <c r="I160" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I46</f>
-        <v>242.15759999999997</v>
+        <f>(($B$142*I$154+$A$142)/100)*I45</f>
+        <v>282.06875999999994</v>
       </c>
       <c r="J160" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J46</f>
-        <v>266.54669999999987</v>
+        <f>(($B$142*J$154+$A$142)/100)*J45</f>
+        <v>309.98393999999985</v>
       </c>
       <c r="K160" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K46</f>
-        <v>305.7195000000001</v>
-      </c>
-      <c r="M160" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K45</f>
+        <v>353.1328400000001</v>
+      </c>
+      <c r="M160" s="54">
         <f t="shared" si="12"/>
-        <v>38.908922911901001</v>
-      </c>
-      <c r="O160" s="49">
-        <v>1.0000000000000001E-15</v>
-      </c>
-      <c r="P160" s="50">
-        <v>0.02</v>
+        <v>46.60176948050119</v>
+      </c>
+      <c r="O160" s="39">
+        <v>9.9999999999999998E-17</v>
+      </c>
+      <c r="P160" s="40">
+        <v>2.1299999999999999E-2</v>
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A161" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B161" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B47</f>
-        <v>110.983</v>
+        <f>(($B$142*B$154+$A$142)/100)*B46</f>
+        <v>126.98519999999999</v>
       </c>
       <c r="C161" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C47</f>
-        <v>117.76589999999997</v>
+        <f>(($B$142*C$154+$A$142)/100)*C46</f>
+        <v>130.68215999999995</v>
       </c>
       <c r="D161" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D47</f>
-        <v>121.97421999999992</v>
+        <f>(($B$142*D$154+$A$142)/100)*D46</f>
+        <v>141.1025599999999</v>
       </c>
       <c r="E161" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E47</f>
-        <v>133.48184000000003</v>
+        <f>(($B$142*E$154+$A$142)/100)*E46</f>
+        <v>151.01960000000003</v>
       </c>
       <c r="F161" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F47</f>
-        <v>145.63139999999999</v>
+        <f>(($B$142*F$154+$A$142)/100)*F46</f>
+        <v>163.53689999999997</v>
       </c>
       <c r="G161" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G47</f>
-        <v>158.5841999999999</v>
+        <f>(($B$142*G$154+$A$142)/100)*G46</f>
+        <v>185.48269999999988</v>
       </c>
       <c r="H161" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H47</f>
-        <v>176.37620000000004</v>
+        <f>(($B$142*H$154+$A$142)/100)*H46</f>
+        <v>197.22066000000007</v>
       </c>
       <c r="I161" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I47</f>
-        <v>190.36277999999999</v>
+        <f>(($B$142*I$154+$A$142)/100)*I46</f>
+        <v>242.15759999999997</v>
       </c>
       <c r="J161" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J47</f>
-        <v>227.71643999999986</v>
+        <f>(($B$142*J$154+$A$142)/100)*J46</f>
+        <v>266.54669999999987</v>
       </c>
       <c r="K161" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K47</f>
-        <v>260.88064000000008</v>
-      </c>
-      <c r="M161" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K46</f>
+        <v>305.7195000000001</v>
+      </c>
+      <c r="M161" s="54">
         <f t="shared" si="12"/>
-        <v>32.485982807963815</v>
-      </c>
-      <c r="O161" s="49">
-        <v>1E-14</v>
-      </c>
-      <c r="P161" s="50">
-        <v>1.8700000000000001E-2</v>
+        <v>38.908922911901001</v>
+      </c>
+      <c r="O161" s="39">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="P161" s="40">
+        <v>0.02</v>
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A162" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B162" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B48</f>
-        <v>94.206500000000005</v>
+        <f>(($B$142*B$154+$A$142)/100)*B47</f>
+        <v>110.983</v>
       </c>
       <c r="C162" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C48</f>
-        <v>102.06377999999997</v>
+        <f>(($B$142*C$154+$A$142)/100)*C47</f>
+        <v>117.76589999999997</v>
       </c>
       <c r="D162" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D48</f>
-        <v>108.80795999999992</v>
+        <f>(($B$142*D$154+$A$142)/100)*D47</f>
+        <v>121.97421999999992</v>
       </c>
       <c r="E162" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E48</f>
-        <v>113.99544000000002</v>
+        <f>(($B$142*E$154+$A$142)/100)*E47</f>
+        <v>133.48184000000003</v>
       </c>
       <c r="F162" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F48</f>
-        <v>126.77093999999997</v>
+        <f>(($B$142*F$154+$A$142)/100)*F47</f>
+        <v>145.63139999999999</v>
       </c>
       <c r="G162" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G48</f>
-        <v>139.40439999999992</v>
+        <f>(($B$142*G$154+$A$142)/100)*G47</f>
+        <v>158.5841999999999</v>
       </c>
       <c r="H162" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H48</f>
-        <v>149.57618000000005</v>
+        <f>(($B$142*H$154+$A$142)/100)*H47</f>
+        <v>176.37620000000004</v>
       </c>
       <c r="I162" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I48</f>
-        <v>168.16499999999999</v>
+        <f>(($B$142*I$154+$A$142)/100)*I47</f>
+        <v>190.36277999999999</v>
       </c>
       <c r="J162" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J48</f>
-        <v>177.69779999999992</v>
+        <f>(($B$142*J$154+$A$142)/100)*J47</f>
+        <v>227.71643999999986</v>
       </c>
       <c r="K162" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K48</f>
-        <v>219.04534000000007</v>
-      </c>
-      <c r="M162" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K47</f>
+        <v>260.88064000000008</v>
+      </c>
+      <c r="M162" s="54">
         <f t="shared" si="12"/>
-        <v>48.105368931368112</v>
-      </c>
-      <c r="O162" s="49">
-        <v>1E-13</v>
-      </c>
-      <c r="P162" s="50">
-        <v>1.77E-2</v>
+        <v>32.485982807963815</v>
+      </c>
+      <c r="O162" s="39">
+        <v>1E-14</v>
+      </c>
+      <c r="P162" s="40">
+        <v>1.8700000000000001E-2</v>
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A163" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B163" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B49</f>
-        <v>75.107100000000003</v>
+        <f>(($B$142*B$154+$A$142)/100)*B48</f>
+        <v>94.206500000000005</v>
       </c>
       <c r="C163" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C49</f>
-        <v>85.60187999999998</v>
+        <f>(($B$142*C$154+$A$142)/100)*C48</f>
+        <v>102.06377999999997</v>
       </c>
       <c r="D163" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D49</f>
-        <v>93.157499999999942</v>
+        <f>(($B$142*D$154+$A$142)/100)*D48</f>
+        <v>108.80795999999992</v>
       </c>
       <c r="E163" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E49</f>
-        <v>100.35496000000002</v>
+        <f>(($B$142*E$154+$A$142)/100)*E48</f>
+        <v>113.99544000000002</v>
       </c>
       <c r="F163" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F49</f>
-        <v>106.71677999999997</v>
+        <f>(($B$142*F$154+$A$142)/100)*F48</f>
+        <v>126.77093999999997</v>
       </c>
       <c r="G163" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G49</f>
-        <v>119.28899999999993</v>
+        <f>(($B$142*G$154+$A$142)/100)*G48</f>
+        <v>139.40439999999992</v>
       </c>
       <c r="H163" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H49</f>
-        <v>129.64796000000004</v>
+        <f>(($B$142*H$154+$A$142)/100)*H48</f>
+        <v>149.57618000000005</v>
       </c>
       <c r="I163" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I49</f>
-        <v>140.58593999999999</v>
+        <f>(($B$142*I$154+$A$142)/100)*I48</f>
+        <v>168.16499999999999</v>
       </c>
       <c r="J163" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J49</f>
-        <v>155.32103999999993</v>
+        <f>(($B$142*J$154+$A$142)/100)*J48</f>
+        <v>177.69779999999992</v>
       </c>
       <c r="K163" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K49</f>
-        <v>167.98482000000004</v>
-      </c>
-      <c r="M163" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K48</f>
+        <v>219.04534000000007</v>
+      </c>
+      <c r="M163" s="54">
         <f t="shared" si="12"/>
-        <v>27.123317738423211</v>
-      </c>
-      <c r="O163" s="49">
+        <v>48.105368931368112</v>
+      </c>
+      <c r="O163" s="39">
         <v>1E-13</v>
       </c>
-      <c r="P163" s="50">
-        <v>1.7399999999999999E-2</v>
+      <c r="P163" s="40">
+        <v>1.77E-2</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A164" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B164" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B50</f>
-        <v>61.427799999999998</v>
+        <f>(($B$142*B$154+$A$142)/100)*B49</f>
+        <v>75.107100000000003</v>
       </c>
       <c r="C164" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C50</f>
-        <v>67.113899999999987</v>
+        <f>(($B$142*C$154+$A$142)/100)*C49</f>
+        <v>85.60187999999998</v>
       </c>
       <c r="D164" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D50</f>
-        <v>76.761779999999945</v>
+        <f>(($B$142*D$154+$A$142)/100)*D49</f>
+        <v>93.157499999999942</v>
       </c>
       <c r="E164" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E50</f>
-        <v>84.278680000000023</v>
+        <f>(($B$142*E$154+$A$142)/100)*E49</f>
+        <v>100.35496000000002</v>
       </c>
       <c r="F164" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F50</f>
-        <v>92.153639999999982</v>
+        <f>(($B$142*F$154+$A$142)/100)*F49</f>
+        <v>106.71677999999997</v>
       </c>
       <c r="G164" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G50</f>
-        <v>98.471899999999934</v>
+        <f>(($B$142*G$154+$A$142)/100)*G49</f>
+        <v>119.28899999999993</v>
       </c>
       <c r="H164" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H50</f>
-        <v>109.26162000000004</v>
+        <f>(($B$142*H$154+$A$142)/100)*H49</f>
+        <v>129.64796000000004</v>
       </c>
       <c r="I164" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I50</f>
-        <v>119.73347999999999</v>
+        <f>(($B$142*I$154+$A$142)/100)*I49</f>
+        <v>140.58593999999999</v>
       </c>
       <c r="J164" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J50</f>
-        <v>127.89853999999993</v>
+        <f>(($B$142*J$154+$A$142)/100)*J49</f>
+        <v>155.32103999999993</v>
       </c>
       <c r="K164" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K50</f>
-        <v>145.02904000000004</v>
-      </c>
-      <c r="M164" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K49</f>
+        <v>167.98482000000004</v>
+      </c>
+      <c r="M164" s="54">
         <f t="shared" si="12"/>
-        <v>26.837729055778073</v>
-      </c>
-      <c r="O164" s="49">
-        <v>1E-14</v>
-      </c>
-      <c r="P164" s="50">
-        <v>1.8599999999999998E-2</v>
+        <v>27.123317738423211</v>
+      </c>
+      <c r="O164" s="39">
+        <v>1E-13</v>
+      </c>
+      <c r="P164" s="40">
+        <v>1.7399999999999999E-2</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A165" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B165" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B51</f>
-        <v>49.813299999999998</v>
+        <f>(($B$142*B$154+$A$142)/100)*B50</f>
+        <v>61.427799999999998</v>
       </c>
       <c r="C165" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C51</f>
-        <v>53.691119999999984</v>
+        <f>(($B$142*C$154+$A$142)/100)*C50</f>
+        <v>67.113899999999987</v>
       </c>
       <c r="D165" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D51</f>
-        <v>59.123959999999961</v>
+        <f>(($B$142*D$154+$A$142)/100)*D50</f>
+        <v>76.761779999999945</v>
       </c>
       <c r="E165" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E51</f>
-        <v>67.958820000000017</v>
+        <f>(($B$142*E$154+$A$142)/100)*E50</f>
+        <v>84.278680000000023</v>
       </c>
       <c r="F165" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F51</f>
-        <v>75.441839999999985</v>
+        <f>(($B$142*F$154+$A$142)/100)*F50</f>
+        <v>92.153639999999982</v>
       </c>
       <c r="G165" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G51</f>
-        <v>82.800599999999946</v>
+        <f>(($B$142*G$154+$A$142)/100)*G50</f>
+        <v>98.471899999999934</v>
       </c>
       <c r="H165" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H51</f>
-        <v>87.95904000000003</v>
+        <f>(($B$142*H$154+$A$142)/100)*H50</f>
+        <v>109.26162000000004</v>
       </c>
       <c r="I165" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I51</f>
-        <v>98.432579999999987</v>
+        <f>(($B$142*I$154+$A$142)/100)*I50</f>
+        <v>119.73347999999999</v>
       </c>
       <c r="J165" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J51</f>
-        <v>107.27681999999994</v>
+        <f>(($B$142*J$154+$A$142)/100)*J50</f>
+        <v>127.89853999999993</v>
       </c>
       <c r="K165" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K51</f>
-        <v>119.71332000000004</v>
-      </c>
-      <c r="M165" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K50</f>
+        <v>145.02904000000004</v>
+      </c>
+      <c r="M165" s="54">
         <f t="shared" si="12"/>
-        <v>18.123756746459325</v>
-      </c>
-      <c r="O165" s="49">
-        <v>1.0000000000000001E-15</v>
-      </c>
-      <c r="P165" s="50">
-        <v>1.9599999999999999E-2</v>
+        <v>26.837729055778073</v>
+      </c>
+      <c r="O165" s="39">
+        <v>1E-14</v>
+      </c>
+      <c r="P165" s="40">
+        <v>1.8599999999999998E-2</v>
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A166" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B166" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B52</f>
-        <v>37.682600000000001</v>
+        <f>(($B$142*B$154+$A$142)/100)*B51</f>
+        <v>49.813299999999998</v>
       </c>
       <c r="C166" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C52</f>
-        <v>42.041159999999991</v>
+        <f>(($B$142*C$154+$A$142)/100)*C51</f>
+        <v>53.691119999999984</v>
       </c>
       <c r="D166" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D52</f>
-        <v>45.460859999999968</v>
+        <f>(($B$142*D$154+$A$142)/100)*D51</f>
+        <v>59.123959999999961</v>
       </c>
       <c r="E166" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E52</f>
-        <v>50.421060000000011</v>
+        <f>(($B$142*E$154+$A$142)/100)*E51</f>
+        <v>67.958820000000017</v>
       </c>
       <c r="F166" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F52</f>
-        <v>58.491299999999988</v>
+        <f>(($B$142*F$154+$A$142)/100)*F51</f>
+        <v>75.441839999999985</v>
       </c>
       <c r="G166" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G52</f>
-        <v>65.258099999999956</v>
+        <f>(($B$142*G$154+$A$142)/100)*G51</f>
+        <v>82.800599999999946</v>
       </c>
       <c r="H166" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H52</f>
-        <v>71.23766000000002</v>
+        <f>(($B$142*H$154+$A$142)/100)*H51</f>
+        <v>87.95904000000003</v>
       </c>
       <c r="I166" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I52</f>
-        <v>76.459019999999995</v>
+        <f>(($B$142*I$154+$A$142)/100)*I51</f>
+        <v>98.432579999999987</v>
       </c>
       <c r="J166" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J52</f>
-        <v>85.996959999999959</v>
+        <f>(($B$142*J$154+$A$142)/100)*J51</f>
+        <v>107.27681999999994</v>
       </c>
       <c r="K166" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K52</f>
-        <v>100.40472000000003</v>
-      </c>
-      <c r="M166" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K51</f>
+        <v>119.71332000000004</v>
+      </c>
+      <c r="M166" s="54">
         <f t="shared" si="12"/>
-        <v>13.980530844150357</v>
-      </c>
-      <c r="O166" s="49">
-        <v>3.0000000000000001E-17</v>
-      </c>
-      <c r="P166" s="50">
-        <v>2.1299999999999999E-2</v>
+        <v>18.123756746459325</v>
+      </c>
+      <c r="O166" s="39">
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="P166" s="40">
+        <v>1.9599999999999999E-2</v>
       </c>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A167" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B167" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B53</f>
-        <v>26.068100000000001</v>
+        <f>(($B$142*B$154+$A$142)/100)*B52</f>
+        <v>37.682600000000001</v>
       </c>
       <c r="C167" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C53</f>
-        <v>29.884679999999992</v>
+        <f>(($B$142*C$154+$A$142)/100)*C52</f>
+        <v>42.041159999999991</v>
       </c>
       <c r="D167" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D53</f>
-        <v>33.536699999999975</v>
+        <f>(($B$142*D$154+$A$142)/100)*D52</f>
+        <v>45.460859999999968</v>
       </c>
       <c r="E167" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E53</f>
-        <v>36.537000000000006</v>
+        <f>(($B$142*E$154+$A$142)/100)*E52</f>
+        <v>50.421060000000011</v>
       </c>
       <c r="F167" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F53</f>
-        <v>40.585799999999992</v>
+        <f>(($B$142*F$154+$A$142)/100)*F52</f>
+        <v>58.491299999999988</v>
       </c>
       <c r="G167" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G53</f>
-        <v>47.481699999999968</v>
+        <f>(($B$142*G$154+$A$142)/100)*G52</f>
+        <v>65.258099999999956</v>
       </c>
       <c r="H167" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H53</f>
-        <v>52.683800000000019</v>
+        <f>(($B$142*H$154+$A$142)/100)*H52</f>
+        <v>71.23766000000002</v>
       </c>
       <c r="I167" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I53</f>
-        <v>58.072979999999994</v>
+        <f>(($B$142*I$154+$A$142)/100)*I52</f>
+        <v>76.459019999999995</v>
       </c>
       <c r="J167" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J53</f>
-        <v>62.962059999999965</v>
+        <f>(($B$142*J$154+$A$142)/100)*J52</f>
+        <v>85.996959999999959</v>
       </c>
       <c r="K167" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K53</f>
-        <v>75.947160000000025</v>
-      </c>
-      <c r="M167" s="65">
+        <f>(($B$142*K$154+$A$142)/100)*K52</f>
+        <v>100.40472000000003</v>
+      </c>
+      <c r="M167" s="54">
         <f t="shared" si="12"/>
-        <v>8.1781693204119676</v>
-      </c>
-      <c r="O167" s="49">
-        <v>1.0000000000000001E-18</v>
-      </c>
-      <c r="P167" s="50">
-        <v>2.2800000000000001E-2</v>
+        <v>13.980530844150357</v>
+      </c>
+      <c r="O167" s="39">
+        <v>3.0000000000000001E-17</v>
+      </c>
+      <c r="P167" s="40">
+        <v>2.1299999999999999E-2</v>
       </c>
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A168" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B168" s="4">
+        <f>(($B$142*B$154+$A$142)/100)*B53</f>
+        <v>26.068100000000001</v>
+      </c>
+      <c r="C168" s="4">
+        <f>(($B$142*C$154+$A$142)/100)*C53</f>
+        <v>29.884679999999992</v>
+      </c>
+      <c r="D168" s="4">
+        <f>(($B$142*D$154+$A$142)/100)*D53</f>
+        <v>33.536699999999975</v>
+      </c>
+      <c r="E168" s="4">
+        <f>(($B$142*E$154+$A$142)/100)*E53</f>
+        <v>36.537000000000006</v>
+      </c>
+      <c r="F168" s="4">
+        <f>(($B$142*F$154+$A$142)/100)*F53</f>
+        <v>40.585799999999992</v>
+      </c>
+      <c r="G168" s="4">
+        <f>(($B$142*G$154+$A$142)/100)*G53</f>
+        <v>47.481699999999968</v>
+      </c>
+      <c r="H168" s="4">
+        <f>(($B$142*H$154+$A$142)/100)*H53</f>
+        <v>52.683800000000019</v>
+      </c>
+      <c r="I168" s="4">
+        <f>(($B$142*I$154+$A$142)/100)*I53</f>
+        <v>58.072979999999994</v>
+      </c>
+      <c r="J168" s="4">
+        <f>(($B$142*J$154+$A$142)/100)*J53</f>
+        <v>62.962059999999965</v>
+      </c>
+      <c r="K168" s="4">
+        <f>(($B$142*K$154+$A$142)/100)*K53</f>
+        <v>75.947160000000025</v>
+      </c>
+      <c r="M168" s="54">
+        <f t="shared" si="12"/>
+        <v>8.1781693204119676</v>
+      </c>
+      <c r="O168" s="39">
+        <v>1.0000000000000001E-18</v>
+      </c>
+      <c r="P168" s="40">
+        <v>2.2800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A169" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B168" s="4">
-        <f>(($B$142*B$153+$A$142)/100)*B54</f>
+      <c r="B169" s="4">
+        <f>(($B$142*B$154+$A$142)/100)*B54</f>
         <v>19.099399999999999</v>
       </c>
-      <c r="C168" s="4">
-        <f>(($B$142*C$153+$A$142)/100)*C54</f>
+      <c r="C169" s="4">
+        <f>(($B$142*C$154+$A$142)/100)*C54</f>
         <v>18.741239999999994</v>
       </c>
-      <c r="D168" s="4">
-        <f>(($B$142*D$153+$A$142)/100)*D54</f>
+      <c r="D169" s="4">
+        <f>(($B$142*D$154+$A$142)/100)*D54</f>
         <v>21.364119999999986</v>
       </c>
-      <c r="E168" s="4">
-        <f>(($B$142*E$153+$A$142)/100)*E54</f>
+      <c r="E169" s="4">
+        <f>(($B$142*E$154+$A$142)/100)*E54</f>
         <v>24.114420000000006</v>
       </c>
-      <c r="F168" s="4">
-        <f>(($B$142*F$153+$A$142)/100)*F54</f>
+      <c r="F169" s="4">
+        <f>(($B$142*F$154+$A$142)/100)*F54</f>
         <v>26.500139999999995</v>
       </c>
-      <c r="G168" s="4">
-        <f>(($B$142*G$153+$A$142)/100)*G54</f>
+      <c r="G169" s="4">
+        <f>(($B$142*G$154+$A$142)/100)*G54</f>
         <v>29.705299999999983</v>
       </c>
-      <c r="H168" s="4">
-        <f>(($B$142*H$153+$A$142)/100)*H54</f>
+      <c r="H169" s="4">
+        <f>(($B$142*H$154+$A$142)/100)*H54</f>
         <v>34.588060000000013</v>
       </c>
-      <c r="I168" s="4">
-        <f>(($B$142*I$153+$A$142)/100)*I54</f>
+      <c r="I169" s="4">
+        <f>(($B$142*I$154+$A$142)/100)*I54</f>
         <v>38.565839999999994</v>
       </c>
-      <c r="J168" s="4">
-        <f>(($B$142*J$153+$A$142)/100)*J54</f>
+      <c r="J169" s="4">
+        <f>(($B$142*J$154+$A$142)/100)*J54</f>
         <v>43.217859999999973</v>
       </c>
-      <c r="K168" s="4">
-        <f>(($B$142*K$153+$A$142)/100)*K54</f>
+      <c r="K169" s="4">
+        <f>(($B$142*K$154+$A$142)/100)*K54</f>
         <v>50.416900000000012</v>
       </c>
-      <c r="M168" s="65">
+      <c r="M169" s="54">
         <f t="shared" si="12"/>
         <v>6.7562521870106114</v>
       </c>
-      <c r="O168" s="49">
+      <c r="O169" s="39">
         <v>1.0000000000000001E-18</v>
       </c>
-      <c r="P168" s="50">
+      <c r="P169" s="40">
         <v>2.2700000000000001E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A169" s="61" t="s">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A170" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B169" s="62">
-        <f>(($B$142*B$153+$A$142)/100)*B55</f>
+      <c r="B170" s="51">
+        <f>(($B$142*B$154+$A$142)/100)*B55</f>
         <v>9.8078000000000003</v>
       </c>
-      <c r="C169" s="62">
-        <f>(($B$142*C$153+$A$142)/100)*C55</f>
+      <c r="C170" s="51">
+        <f>(($B$142*C$154+$A$142)/100)*C55</f>
         <v>11.649959999999997</v>
       </c>
-      <c r="D169" s="62">
-        <f>(($B$142*D$153+$A$142)/100)*D55</f>
+      <c r="D170" s="51">
+        <f>(($B$142*D$154+$A$142)/100)*D55</f>
         <v>11.178899999999993</v>
       </c>
-      <c r="E169" s="62">
-        <f>(($B$142*E$153+$A$142)/100)*E55</f>
+      <c r="E170" s="51">
+        <f>(($B$142*E$154+$A$142)/100)*E55</f>
         <v>12.909740000000003</v>
       </c>
-      <c r="F169" s="62">
-        <f>(($B$142*F$153+$A$142)/100)*F55</f>
+      <c r="F170" s="51">
+        <f>(($B$142*F$154+$A$142)/100)*F55</f>
         <v>14.801879999999997</v>
       </c>
-      <c r="G169" s="62">
-        <f>(($B$142*G$153+$A$142)/100)*G55</f>
+      <c r="G170" s="51">
+        <f>(($B$142*G$154+$A$142)/100)*G55</f>
         <v>16.139099999999988</v>
       </c>
-      <c r="H169" s="62">
-        <f>(($B$142*H$153+$A$142)/100)*H55</f>
+      <c r="H170" s="51">
+        <f>(($B$142*H$154+$A$142)/100)*H55</f>
         <v>18.095740000000006</v>
       </c>
-      <c r="I169" s="62">
-        <f>(($B$142*I$153+$A$142)/100)*I55</f>
+      <c r="I170" s="51">
+        <f>(($B$142*I$154+$A$142)/100)*I55</f>
         <v>21.300899999999999</v>
       </c>
-      <c r="J169" s="62">
-        <f>(($B$142*J$153+$A$142)/100)*J55</f>
+      <c r="J170" s="51">
+        <f>(($B$142*J$154+$A$142)/100)*J55</f>
         <v>24.351179999999985</v>
       </c>
-      <c r="K169" s="62">
-        <f>(($B$142*K$153+$A$142)/100)*K55</f>
+      <c r="K170" s="51">
+        <f>(($B$142*K$154+$A$142)/100)*K55</f>
         <v>28.962900000000008</v>
       </c>
-      <c r="M169" s="65">
+      <c r="M170" s="54">
         <f t="shared" si="12"/>
         <v>4.250473607017895</v>
       </c>
-      <c r="O169" s="49">
+      <c r="O170" s="39">
         <v>2E-19</v>
       </c>
-      <c r="P169" s="50">
+      <c r="P170" s="40">
         <v>2.3300000000000001E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A170" s="59"/>
-      <c r="B170" s="63">
-        <f>SUM(B154:B167)</f>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A171" s="48"/>
+      <c r="B171" s="52">
+        <f>SUM(B155:B168)</f>
         <v>1733.1415</v>
       </c>
-      <c r="C170" s="63">
-        <f t="shared" ref="C170:K170" si="13">SUM(C154:C167)</f>
+      <c r="C171" s="52">
+        <f t="shared" ref="C171:K171" si="13">SUM(C155:C168)</f>
         <v>1890.8391599999991</v>
       </c>
-      <c r="D170" s="63">
+      <c r="D171" s="52">
         <f t="shared" si="13"/>
         <v>2078.2817199999986</v>
       </c>
-      <c r="E170" s="63">
+      <c r="E171" s="52">
         <f t="shared" si="13"/>
         <v>2304.5103799999997</v>
       </c>
-      <c r="F170" s="63">
+      <c r="F171" s="52">
         <f t="shared" si="13"/>
         <v>2573.6171999999992</v>
       </c>
-      <c r="G170" s="63">
+      <c r="G171" s="52">
         <f t="shared" si="13"/>
         <v>2882.3496999999979</v>
       </c>
-      <c r="H170" s="63">
+      <c r="H171" s="52">
         <f t="shared" si="13"/>
         <v>3195.6160600000021</v>
       </c>
-      <c r="I170" s="63">
+      <c r="I171" s="52">
         <f t="shared" si="13"/>
         <v>3581.9144999999994</v>
       </c>
-      <c r="J170" s="63">
+      <c r="J171" s="52">
         <f t="shared" si="13"/>
         <v>3930.8508399999982</v>
       </c>
-      <c r="K170" s="63">
+      <c r="K171" s="52">
         <f t="shared" si="13"/>
         <v>4294.0181000000021</v>
       </c>
-      <c r="M170" s="56">
-        <f>SUM(M154:M167)</f>
+      <c r="M171" s="45">
+        <f>SUM(M155:M168)</f>
         <v>652.27230315014242</v>
       </c>
-    </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B171" s="53"/>
-      <c r="C171" s="53"/>
-      <c r="D171" s="53"/>
-      <c r="E171" s="53"/>
-      <c r="F171" s="53"/>
-      <c r="G171" s="53"/>
-      <c r="H171" s="53"/>
-      <c r="I171" s="53"/>
-      <c r="J171" s="53"/>
-      <c r="K171" s="53"/>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A172" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B172" s="51"/>
-      <c r="C172" s="51"/>
-      <c r="D172" s="51"/>
-      <c r="E172" s="51"/>
-      <c r="F172" s="51"/>
-      <c r="G172" s="51"/>
-      <c r="H172" s="51"/>
-      <c r="I172" s="51"/>
-      <c r="J172" s="51"/>
-      <c r="K172" s="51"/>
+      <c r="B172" s="42"/>
+      <c r="C172" s="42"/>
+      <c r="D172" s="42"/>
+      <c r="E172" s="42"/>
+      <c r="F172" s="42"/>
+      <c r="G172" s="42"/>
+      <c r="H172" s="42"/>
+      <c r="I172" s="42"/>
+      <c r="J172" s="42"/>
+      <c r="K172" s="42"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A173" s="4"/>
-      <c r="B173" s="7">
-        <v>1950</v>
-      </c>
-      <c r="C173" s="7">
-        <v>1955</v>
-      </c>
-      <c r="D173" s="7">
-        <v>1960</v>
-      </c>
-      <c r="E173" s="7">
-        <v>1965</v>
-      </c>
-      <c r="F173" s="7">
-        <v>1970</v>
-      </c>
-      <c r="G173" s="7">
-        <v>1975</v>
-      </c>
-      <c r="H173" s="7">
-        <v>1980</v>
-      </c>
-      <c r="I173" s="7">
-        <v>1985</v>
-      </c>
-      <c r="J173" s="7">
-        <v>1990</v>
-      </c>
-      <c r="K173" s="7">
-        <v>1995</v>
-      </c>
-      <c r="M173" s="27">
-        <v>1910</v>
-      </c>
-      <c r="N173" s="54"/>
-      <c r="O173" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="P173" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="A173" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B173" s="55"/>
+      <c r="C173" s="55"/>
+      <c r="D173" s="55"/>
+      <c r="E173" s="55"/>
+      <c r="F173" s="55"/>
+      <c r="G173" s="55"/>
+      <c r="H173" s="55"/>
+      <c r="I173" s="55"/>
+      <c r="J173" s="55"/>
+      <c r="K173" s="55"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A174" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B174" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B60</f>
-        <v>260.68099999999998</v>
-      </c>
-      <c r="C174" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C60</f>
-        <v>316.57499999999993</v>
-      </c>
-      <c r="D174" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D60</f>
-        <v>350.52061999999978</v>
-      </c>
-      <c r="E174" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E60</f>
-        <v>385.34356000000008</v>
-      </c>
-      <c r="F174" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F60</f>
-        <v>419.7049199999999</v>
-      </c>
-      <c r="G174" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G60</f>
-        <v>463.82369999999975</v>
-      </c>
-      <c r="H174" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H60</f>
-        <v>502.09952000000015</v>
-      </c>
-      <c r="I174" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I60</f>
-        <v>569.51879999999994</v>
-      </c>
-      <c r="J174" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J60</f>
-        <v>589.03529999999967</v>
-      </c>
-      <c r="K174" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K60</f>
-        <v>542.57166000000018</v>
-      </c>
-      <c r="M174" s="65">
-        <f>O174*EXP($M$173*P174)</f>
-        <v>156.85219677743601</v>
-      </c>
-      <c r="N174" s="55"/>
-      <c r="O174" s="49">
-        <v>7.0000000000000005E-13</v>
-      </c>
-      <c r="P174" s="50">
-        <v>1.7299999999999999E-2</v>
+      <c r="A174" s="4"/>
+      <c r="B174" s="7">
+        <v>1950</v>
+      </c>
+      <c r="C174" s="7">
+        <v>1955</v>
+      </c>
+      <c r="D174" s="7">
+        <v>1960</v>
+      </c>
+      <c r="E174" s="7">
+        <v>1965</v>
+      </c>
+      <c r="F174" s="7">
+        <v>1970</v>
+      </c>
+      <c r="G174" s="7">
+        <v>1975</v>
+      </c>
+      <c r="H174" s="7">
+        <v>1980</v>
+      </c>
+      <c r="I174" s="7">
+        <v>1985</v>
+      </c>
+      <c r="J174" s="7">
+        <v>1990</v>
+      </c>
+      <c r="K174" s="7">
+        <v>1995</v>
+      </c>
+      <c r="M174" s="27">
+        <v>1910</v>
+      </c>
+      <c r="N174" s="43"/>
+      <c r="O174" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P174" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A175" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B175" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B61</f>
-        <v>219.38499999999999</v>
+        <f>(($B$142*B$174+$A$142)/100)*B60</f>
+        <v>260.68099999999998</v>
       </c>
       <c r="C175" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C61</f>
-        <v>235.78505999999993</v>
+        <f>(($B$142*C$174+$A$142)/100)*C60</f>
+        <v>316.57499999999993</v>
       </c>
       <c r="D175" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D61</f>
-        <v>290.6513999999998</v>
+        <f>(($B$142*D$174+$A$142)/100)*D60</f>
+        <v>350.52061999999978</v>
       </c>
       <c r="E175" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E61</f>
-        <v>324.44856000000004</v>
+        <f>(($B$142*E$174+$A$142)/100)*E60</f>
+        <v>385.34356000000008</v>
       </c>
       <c r="F175" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F61</f>
-        <v>359.78117999999995</v>
+        <f>(($B$142*F$174+$A$142)/100)*F60</f>
+        <v>419.7049199999999</v>
       </c>
       <c r="G175" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G61</f>
-        <v>396.46049999999974</v>
+        <f>(($B$142*G$174+$A$142)/100)*G60</f>
+        <v>463.82369999999975</v>
       </c>
       <c r="H175" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H61</f>
-        <v>442.08580000000012</v>
+        <f>(($B$142*H$174+$A$142)/100)*H60</f>
+        <v>502.09952000000015</v>
       </c>
       <c r="I175" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I61</f>
-        <v>482.07299999999992</v>
+        <f>(($B$142*I$174+$A$142)/100)*I60</f>
+        <v>569.51879999999994</v>
       </c>
       <c r="J175" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J61</f>
-        <v>548.0112399999997</v>
+        <f>(($B$142*J$174+$A$142)/100)*J60</f>
+        <v>589.03529999999967</v>
       </c>
       <c r="K175" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K61</f>
-        <v>568.74554000000012</v>
-      </c>
-      <c r="M175" s="65">
-        <f t="shared" ref="M175:M189" si="14">O175*EXP($M$173*P175)</f>
-        <v>102.61289100384487</v>
-      </c>
-      <c r="N175" s="19"/>
-      <c r="O175" s="49">
-        <v>7.0000000000000003E-17</v>
-      </c>
-      <c r="P175" s="50">
-        <v>2.1899999999999999E-2</v>
+        <f>(($B$142*K$174+$A$142)/100)*K60</f>
+        <v>542.57166000000018</v>
+      </c>
+      <c r="M175" s="54">
+        <f>O175*EXP($M$174*P175)</f>
+        <v>156.85219677743601</v>
+      </c>
+      <c r="N175" s="44"/>
+      <c r="O175" s="39">
+        <v>7.0000000000000005E-13</v>
+      </c>
+      <c r="P175" s="40">
+        <v>1.7299999999999999E-2</v>
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A176" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B176" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B62</f>
-        <v>191.5102</v>
+        <f>(($B$142*B$174+$A$142)/100)*B61</f>
+        <v>219.38499999999999</v>
       </c>
       <c r="C176" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C62</f>
-        <v>208.93949999999995</v>
+        <f>(($B$142*C$174+$A$142)/100)*C61</f>
+        <v>235.78505999999993</v>
       </c>
       <c r="D176" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D62</f>
-        <v>225.81377999999984</v>
+        <f>(($B$142*D$174+$A$142)/100)*D61</f>
+        <v>290.6513999999998</v>
       </c>
       <c r="E176" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E62</f>
-        <v>279.14268000000004</v>
+        <f>(($B$142*E$174+$A$142)/100)*E61</f>
+        <v>324.44856000000004</v>
       </c>
       <c r="F176" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F62</f>
-        <v>312.51065999999992</v>
+        <f>(($B$142*F$174+$A$142)/100)*F61</f>
+        <v>359.78117999999995</v>
       </c>
       <c r="G176" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G62</f>
-        <v>348.04319999999979</v>
+        <f>(($B$142*G$174+$A$142)/100)*G61</f>
+        <v>396.46049999999974</v>
       </c>
       <c r="H176" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H62</f>
-        <v>383.67550000000011</v>
+        <f>(($B$142*H$174+$A$142)/100)*H61</f>
+        <v>442.08580000000012</v>
       </c>
       <c r="I176" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I62</f>
-        <v>428.70863999999995</v>
+        <f>(($B$142*I$174+$A$142)/100)*I61</f>
+        <v>482.07299999999992</v>
       </c>
       <c r="J176" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J62</f>
-        <v>467.06001999999972</v>
+        <f>(($B$142*J$174+$A$142)/100)*J61</f>
+        <v>548.0112399999997</v>
       </c>
       <c r="K176" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K62</f>
-        <v>532.7028200000002</v>
-      </c>
-      <c r="M176" s="65">
-        <f t="shared" si="14"/>
-        <v>87.786369045850634</v>
-      </c>
-      <c r="O176" s="49">
-        <v>5.0000000000000004E-18</v>
-      </c>
-      <c r="P176" s="50">
-        <v>2.3199999999999998E-2</v>
+        <f>(($B$142*K$174+$A$142)/100)*K61</f>
+        <v>568.74554000000012</v>
+      </c>
+      <c r="M176" s="54">
+        <f t="shared" ref="M176:M190" si="14">O176*EXP($M$174*P176)</f>
+        <v>102.61289100384487</v>
+      </c>
+      <c r="N176" s="19"/>
+      <c r="O176" s="39">
+        <v>7.0000000000000003E-17</v>
+      </c>
+      <c r="P176" s="40">
+        <v>2.1899999999999999E-2</v>
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A177" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B177" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B63</f>
-        <v>167.76499999999999</v>
+        <f>(($B$142*B$174+$A$142)/100)*B62</f>
+        <v>191.5102</v>
       </c>
       <c r="C177" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C63</f>
-        <v>183.61349999999996</v>
+        <f>(($B$142*C$174+$A$142)/100)*C62</f>
+        <v>208.93949999999995</v>
       </c>
       <c r="D177" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D63</f>
-        <v>201.22019999999986</v>
+        <f>(($B$142*D$174+$A$142)/100)*D62</f>
+        <v>225.81377999999984</v>
       </c>
       <c r="E177" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E63</f>
-        <v>218.00410000000005</v>
+        <f>(($B$142*E$174+$A$142)/100)*E62</f>
+        <v>279.14268000000004</v>
       </c>
       <c r="F177" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F63</f>
-        <v>270.01493999999997</v>
+        <f>(($B$142*F$174+$A$142)/100)*F62</f>
+        <v>312.51065999999992</v>
       </c>
       <c r="G177" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G63</f>
-        <v>303.1343999999998</v>
+        <f>(($B$142*G$174+$A$142)/100)*G62</f>
+        <v>348.04319999999979</v>
       </c>
       <c r="H177" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H63</f>
-        <v>337.40538000000009</v>
+        <f>(($B$142*H$174+$A$142)/100)*H62</f>
+        <v>383.67550000000011</v>
       </c>
       <c r="I177" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I63</f>
-        <v>372.87785999999994</v>
+        <f>(($B$142*I$174+$A$142)/100)*I62</f>
+        <v>428.70863999999995</v>
       </c>
       <c r="J177" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J63</f>
-        <v>415.72509999999977</v>
+        <f>(($B$142*J$174+$A$142)/100)*J62</f>
+        <v>467.06001999999972</v>
       </c>
       <c r="K177" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K63</f>
-        <v>456.54112000000015</v>
-      </c>
-      <c r="M177" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K62</f>
+        <v>532.7028200000002</v>
+      </c>
+      <c r="M177" s="54">
         <f t="shared" si="14"/>
-        <v>63.757104105268432</v>
-      </c>
-      <c r="O177" s="49">
-        <v>2.9999999999999998E-18</v>
-      </c>
-      <c r="P177" s="50">
-        <v>2.3300000000000001E-2</v>
+        <v>87.786369045850634</v>
+      </c>
+      <c r="O177" s="39">
+        <v>5.0000000000000004E-18</v>
+      </c>
+      <c r="P177" s="40">
+        <v>2.3199999999999998E-2</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A178" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B178" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B64</f>
-        <v>149.69800000000001</v>
+        <f>(($B$142*B$174+$A$142)/100)*B63</f>
+        <v>167.76499999999999</v>
       </c>
       <c r="C178" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C64</f>
-        <v>160.56683999999996</v>
+        <f>(($B$142*C$174+$A$142)/100)*C63</f>
+        <v>183.61349999999996</v>
       </c>
       <c r="D178" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D64</f>
-        <v>176.37819999999988</v>
+        <f>(($B$142*D$174+$A$142)/100)*D63</f>
+        <v>201.22019999999986</v>
       </c>
       <c r="E178" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E64</f>
-        <v>194.86400000000003</v>
+        <f>(($B$142*E$174+$A$142)/100)*E63</f>
+        <v>218.00410000000005</v>
       </c>
       <c r="F178" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F64</f>
-        <v>212.00111999999996</v>
+        <f>(($B$142*F$174+$A$142)/100)*F63</f>
+        <v>270.01493999999997</v>
       </c>
       <c r="G178" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G64</f>
-        <v>262.20189999999985</v>
+        <f>(($B$142*G$174+$A$142)/100)*G63</f>
+        <v>303.1343999999998</v>
       </c>
       <c r="H178" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H64</f>
-        <v>293.42586000000011</v>
+        <f>(($B$142*H$174+$A$142)/100)*H63</f>
+        <v>337.40538000000009</v>
       </c>
       <c r="I178" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I64</f>
-        <v>327.80963999999994</v>
+        <f>(($B$142*I$174+$A$142)/100)*I63</f>
+        <v>372.87785999999994</v>
       </c>
       <c r="J178" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J64</f>
-        <v>360.6607199999998</v>
+        <f>(($B$142*J$174+$A$142)/100)*J63</f>
+        <v>415.72509999999977</v>
       </c>
       <c r="K178" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K64</f>
-        <v>412.34588000000014</v>
-      </c>
-      <c r="M178" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K63</f>
+        <v>456.54112000000015</v>
+      </c>
+      <c r="M178" s="54">
         <f t="shared" si="14"/>
-        <v>51.450259534369195</v>
-      </c>
-      <c r="O178" s="49">
-        <v>2.0000000000000001E-18</v>
-      </c>
-      <c r="P178" s="50">
-        <v>2.3400000000000001E-2</v>
+        <v>63.757104105268432</v>
+      </c>
+      <c r="O178" s="39">
+        <v>2.9999999999999998E-18</v>
+      </c>
+      <c r="P178" s="40">
+        <v>2.3300000000000001E-2</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A179" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B179" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B65</f>
-        <v>131.631</v>
+        <f>(($B$142*B$174+$A$142)/100)*B64</f>
+        <v>149.69800000000001</v>
       </c>
       <c r="C179" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C65</f>
-        <v>142.58537999999996</v>
+        <f>(($B$142*C$174+$A$142)/100)*C64</f>
+        <v>160.56683999999996</v>
       </c>
       <c r="D179" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D65</f>
-        <v>153.52355999999989</v>
+        <f>(($B$142*D$174+$A$142)/100)*D64</f>
+        <v>176.37819999999988</v>
       </c>
       <c r="E179" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E65</f>
-        <v>170.74958000000004</v>
+        <f>(($B$142*E$174+$A$142)/100)*E64</f>
+        <v>194.86400000000003</v>
       </c>
       <c r="F179" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F65</f>
-        <v>189.55955999999998</v>
+        <f>(($B$142*F$174+$A$142)/100)*F64</f>
+        <v>212.00111999999996</v>
       </c>
       <c r="G179" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G65</f>
-        <v>206.06589999999989</v>
+        <f>(($B$142*G$174+$A$142)/100)*G64</f>
+        <v>262.20189999999985</v>
       </c>
       <c r="H179" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H65</f>
-        <v>252.88224000000008</v>
+        <f>(($B$142*H$174+$A$142)/100)*H64</f>
+        <v>293.42586000000011</v>
       </c>
       <c r="I179" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I65</f>
-        <v>284.75939999999997</v>
+        <f>(($B$142*I$174+$A$142)/100)*I64</f>
+        <v>327.80963999999994</v>
       </c>
       <c r="J179" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J65</f>
-        <v>315.68781999999982</v>
+        <f>(($B$142*J$174+$A$142)/100)*J64</f>
+        <v>360.6607199999998</v>
       </c>
       <c r="K179" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K65</f>
-        <v>363.43076000000013</v>
-      </c>
-      <c r="M179" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K64</f>
+        <v>412.34588000000014</v>
+      </c>
+      <c r="M179" s="54">
         <f t="shared" si="14"/>
-        <v>43.513908158546549</v>
-      </c>
-      <c r="O179" s="49">
-        <v>2.9999999999999998E-18</v>
-      </c>
-      <c r="P179" s="50">
-        <v>2.3099999999999999E-2</v>
+        <v>51.450259534369195</v>
+      </c>
+      <c r="O179" s="39">
+        <v>2.0000000000000001E-18</v>
+      </c>
+      <c r="P179" s="40">
+        <v>2.3400000000000001E-2</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A180" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B180" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B66</f>
-        <v>121.307</v>
+        <f>(($B$142*B$174+$A$142)/100)*B65</f>
+        <v>131.631</v>
       </c>
       <c r="C180" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C66</f>
-        <v>124.85717999999997</v>
+        <f>(($B$142*C$174+$A$142)/100)*C65</f>
+        <v>142.58537999999996</v>
       </c>
       <c r="D180" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D66</f>
-        <v>135.88573999999991</v>
+        <f>(($B$142*D$174+$A$142)/100)*D65</f>
+        <v>153.52355999999989</v>
       </c>
       <c r="E180" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E66</f>
-        <v>148.09664000000004</v>
+        <f>(($B$142*E$174+$A$142)/100)*E65</f>
+        <v>170.74958000000004</v>
       </c>
       <c r="F180" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F66</f>
-        <v>165.44681999999997</v>
+        <f>(($B$142*F$174+$A$142)/100)*F65</f>
+        <v>189.55955999999998</v>
       </c>
       <c r="G180" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G66</f>
-        <v>184.07929999999988</v>
+        <f>(($B$142*G$174+$A$142)/100)*G65</f>
+        <v>206.06589999999989</v>
       </c>
       <c r="H180" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H66</f>
-        <v>198.13690000000005</v>
+        <f>(($B$142*H$174+$A$142)/100)*H65</f>
+        <v>252.88224000000008</v>
       </c>
       <c r="I180" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I66</f>
-        <v>244.62401999999997</v>
+        <f>(($B$142*I$174+$A$142)/100)*I65</f>
+        <v>284.75939999999997</v>
       </c>
       <c r="J180" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J66</f>
-        <v>273.34747999999985</v>
+        <f>(($B$142*J$174+$A$142)/100)*J65</f>
+        <v>315.68781999999982</v>
       </c>
       <c r="K180" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K66</f>
-        <v>319.66460000000012</v>
-      </c>
-      <c r="M180" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K65</f>
+        <v>363.43076000000013</v>
+      </c>
+      <c r="M180" s="54">
         <f t="shared" si="14"/>
-        <v>53.232318780424968</v>
-      </c>
-      <c r="O180" s="49">
-        <v>3.0000000000000001E-17</v>
-      </c>
-      <c r="P180" s="50">
-        <v>2.1999999999999999E-2</v>
+        <v>43.513908158546549</v>
+      </c>
+      <c r="O180" s="39">
+        <v>2.9999999999999998E-18</v>
+      </c>
+      <c r="P180" s="40">
+        <v>2.3099999999999999E-2</v>
       </c>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A181" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B181" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B67</f>
-        <v>101.9495</v>
+        <f>(($B$142*B$174+$A$142)/100)*B66</f>
+        <v>121.307</v>
       </c>
       <c r="C181" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C67</f>
-        <v>114.47351999999997</v>
+        <f>(($B$142*C$174+$A$142)/100)*C66</f>
+        <v>124.85717999999997</v>
       </c>
       <c r="D181" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D67</f>
-        <v>118.24791999999992</v>
+        <f>(($B$142*D$174+$A$142)/100)*D66</f>
+        <v>135.88573999999991</v>
       </c>
       <c r="E181" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E67</f>
-        <v>130.07172000000003</v>
+        <f>(($B$142*E$174+$A$142)/100)*E66</f>
+        <v>148.09664000000004</v>
       </c>
       <c r="F181" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F67</f>
-        <v>142.76651999999996</v>
+        <f>(($B$142*F$174+$A$142)/100)*F66</f>
+        <v>165.44681999999997</v>
       </c>
       <c r="G181" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G67</f>
-        <v>159.51979999999989</v>
+        <f>(($B$142*G$174+$A$142)/100)*G66</f>
+        <v>184.07929999999988</v>
       </c>
       <c r="H181" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H67</f>
-        <v>175.91808000000006</v>
+        <f>(($B$142*H$174+$A$142)/100)*H66</f>
+        <v>198.13690000000005</v>
       </c>
       <c r="I181" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I67</f>
-        <v>190.81121999999999</v>
+        <f>(($B$142*I$174+$A$142)/100)*I66</f>
+        <v>244.62401999999997</v>
       </c>
       <c r="J181" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J67</f>
-        <v>234.07845999999986</v>
+        <f>(($B$142*J$174+$A$142)/100)*J66</f>
+        <v>273.34747999999985</v>
       </c>
       <c r="K181" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K67</f>
-        <v>275.89844000000011</v>
-      </c>
-      <c r="M181" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K66</f>
+        <v>319.66460000000012</v>
+      </c>
+      <c r="M181" s="54">
         <f t="shared" si="14"/>
-        <v>31.805477141060052</v>
-      </c>
-      <c r="O181" s="49">
-        <v>9.9999999999999998E-17</v>
-      </c>
-      <c r="P181" s="50">
-        <v>2.1100000000000001E-2</v>
+        <v>53.232318780424968</v>
+      </c>
+      <c r="O181" s="39">
+        <v>3.0000000000000001E-17</v>
+      </c>
+      <c r="P181" s="40">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A182" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B182" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B68</f>
-        <v>90.334999999999994</v>
+        <f>(($B$142*B$174+$A$142)/100)*B67</f>
+        <v>101.9495</v>
       </c>
       <c r="C182" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C68</f>
-        <v>95.732279999999975</v>
+        <f>(($B$142*C$174+$A$142)/100)*C67</f>
+        <v>114.47351999999997</v>
       </c>
       <c r="D182" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D68</f>
-        <v>107.81427999999993</v>
+        <f>(($B$142*D$174+$A$142)/100)*D67</f>
+        <v>118.24791999999992</v>
       </c>
       <c r="E182" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E68</f>
-        <v>112.29038000000003</v>
+        <f>(($B$142*E$174+$A$142)/100)*E67</f>
+        <v>130.07172000000003</v>
       </c>
       <c r="F182" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F68</f>
-        <v>124.38353999999998</v>
+        <f>(($B$142*F$174+$A$142)/100)*F67</f>
+        <v>142.76651999999996</v>
       </c>
       <c r="G182" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G68</f>
-        <v>136.59759999999991</v>
+        <f>(($B$142*G$174+$A$142)/100)*G67</f>
+        <v>159.51979999999989</v>
       </c>
       <c r="H182" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H68</f>
-        <v>151.40866000000005</v>
+        <f>(($B$142*H$174+$A$142)/100)*H67</f>
+        <v>175.91808000000006</v>
       </c>
       <c r="I182" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I68</f>
-        <v>167.94077999999999</v>
+        <f>(($B$142*I$174+$A$142)/100)*I67</f>
+        <v>190.81121999999999</v>
       </c>
       <c r="J182" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J68</f>
-        <v>181.86601999999991</v>
+        <f>(($B$142*J$174+$A$142)/100)*J67</f>
+        <v>234.07845999999986</v>
       </c>
       <c r="K182" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K68</f>
-        <v>234.06314000000006</v>
-      </c>
-      <c r="M182" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K67</f>
+        <v>275.89844000000011</v>
+      </c>
+      <c r="M182" s="54">
         <f t="shared" si="14"/>
-        <v>43.876145321947618</v>
-      </c>
-      <c r="O182" s="49">
-        <v>2.0000000000000002E-15</v>
-      </c>
-      <c r="P182" s="50">
-        <v>1.9699999999999999E-2</v>
+        <v>31.805477141060052</v>
+      </c>
+      <c r="O182" s="39">
+        <v>9.9999999999999998E-17</v>
+      </c>
+      <c r="P182" s="40">
+        <v>2.1100000000000001E-2</v>
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A183" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B183" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B69</f>
-        <v>70.977499999999992</v>
+        <f>(($B$142*B$174+$A$142)/100)*B68</f>
+        <v>90.334999999999994</v>
       </c>
       <c r="C183" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C69</f>
-        <v>84.335579999999979</v>
+        <f>(($B$142*C$174+$A$142)/100)*C68</f>
+        <v>95.732279999999975</v>
       </c>
       <c r="D183" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D69</f>
-        <v>89.431199999999947</v>
+        <f>(($B$142*D$174+$A$142)/100)*D68</f>
+        <v>107.81427999999993</v>
       </c>
       <c r="E183" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E69</f>
-        <v>101.57286000000002</v>
+        <f>(($B$142*E$174+$A$142)/100)*E68</f>
+        <v>112.29038000000003</v>
       </c>
       <c r="F183" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F69</f>
-        <v>106.23929999999999</v>
+        <f>(($B$142*F$174+$A$142)/100)*F68</f>
+        <v>124.38353999999998</v>
       </c>
       <c r="G183" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G69</f>
-        <v>118.11949999999993</v>
+        <f>(($B$142*G$174+$A$142)/100)*G68</f>
+        <v>136.59759999999991</v>
       </c>
       <c r="H183" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H69</f>
-        <v>128.73172000000005</v>
+        <f>(($B$142*H$174+$A$142)/100)*H68</f>
+        <v>151.40866000000005</v>
       </c>
       <c r="I183" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I69</f>
-        <v>143.50079999999997</v>
+        <f>(($B$142*I$174+$A$142)/100)*I68</f>
+        <v>167.94077999999999</v>
       </c>
       <c r="J183" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J69</f>
-        <v>159.26987999999992</v>
+        <f>(($B$142*J$174+$A$142)/100)*J68</f>
+        <v>181.86601999999991</v>
       </c>
       <c r="K183" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K69</f>
-        <v>181.50084000000007</v>
-      </c>
-      <c r="M183" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K68</f>
+        <v>234.06314000000006</v>
+      </c>
+      <c r="M183" s="54">
         <f t="shared" si="14"/>
-        <v>29.945252135950131</v>
-      </c>
-      <c r="O183" s="49">
+        <v>43.876145321947618</v>
+      </c>
+      <c r="O183" s="39">
         <v>2.0000000000000002E-15</v>
       </c>
-      <c r="P183" s="50">
-        <v>1.95E-2</v>
+      <c r="P183" s="40">
+        <v>1.9699999999999999E-2</v>
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A184" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B184" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B70</f>
-        <v>64.525000000000006</v>
+        <f>(($B$142*B$174+$A$142)/100)*B69</f>
+        <v>70.977499999999992</v>
       </c>
       <c r="C184" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C70</f>
-        <v>65.594339999999988</v>
+        <f>(($B$142*C$174+$A$142)/100)*C69</f>
+        <v>84.335579999999979</v>
       </c>
       <c r="D184" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D70</f>
-        <v>78.252299999999948</v>
+        <f>(($B$142*D$174+$A$142)/100)*D69</f>
+        <v>89.431199999999947</v>
       </c>
       <c r="E184" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E70</f>
-        <v>83.547940000000011</v>
+        <f>(($B$142*E$174+$A$142)/100)*E69</f>
+        <v>101.57286000000002</v>
       </c>
       <c r="F184" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F70</f>
-        <v>95.018519999999981</v>
+        <f>(($B$142*F$174+$A$142)/100)*F69</f>
+        <v>106.23929999999999</v>
       </c>
       <c r="G184" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G70</f>
-        <v>99.641399999999933</v>
+        <f>(($B$142*G$174+$A$142)/100)*G69</f>
+        <v>118.11949999999993</v>
       </c>
       <c r="H184" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H70</f>
-        <v>110.17786000000004</v>
+        <f>(($B$142*H$174+$A$142)/100)*H69</f>
+        <v>128.73172000000005</v>
       </c>
       <c r="I184" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I70</f>
-        <v>120.85457999999998</v>
+        <f>(($B$142*I$174+$A$142)/100)*I69</f>
+        <v>143.50079999999997</v>
       </c>
       <c r="J184" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J70</f>
-        <v>135.13807999999992</v>
+        <f>(($B$142*J$174+$A$142)/100)*J69</f>
+        <v>159.26987999999992</v>
       </c>
       <c r="K184" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K70</f>
-        <v>158.54506000000003</v>
-      </c>
-      <c r="M184" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K69</f>
+        <v>181.50084000000007</v>
+      </c>
+      <c r="M184" s="54">
         <f t="shared" si="14"/>
-        <v>18.123756746459325</v>
-      </c>
-      <c r="O184" s="4">
-        <f xml:space="preserve"> 0.000000000000001</f>
-        <v>1.0000000000000001E-15</v>
-      </c>
-      <c r="P184" s="50">
-        <v>1.9599999999999999E-2</v>
+        <v>29.945252135950131</v>
+      </c>
+      <c r="O184" s="39">
+        <v>2.0000000000000002E-15</v>
+      </c>
+      <c r="P184" s="40">
+        <v>1.95E-2</v>
       </c>
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A185" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B185" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B71</f>
-        <v>51.62</v>
+        <f>(($B$142*B$174+$A$142)/100)*B70</f>
+        <v>64.525000000000006</v>
       </c>
       <c r="C185" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C71</f>
-        <v>58.503059999999984</v>
+        <f>(($B$142*C$174+$A$142)/100)*C70</f>
+        <v>65.594339999999988</v>
       </c>
       <c r="D185" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D71</f>
-        <v>59.62079999999996</v>
+        <f>(($B$142*D$174+$A$142)/100)*D70</f>
+        <v>78.252299999999948</v>
       </c>
       <c r="E185" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E71</f>
-        <v>71.368940000000009</v>
+        <f>(($B$142*E$174+$A$142)/100)*E70</f>
+        <v>83.547940000000011</v>
       </c>
       <c r="F185" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F71</f>
-        <v>76.635539999999992</v>
+        <f>(($B$142*F$174+$A$142)/100)*F70</f>
+        <v>95.018519999999981</v>
       </c>
       <c r="G185" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G71</f>
-        <v>87.478599999999943</v>
+        <f>(($B$142*G$174+$A$142)/100)*G70</f>
+        <v>99.641399999999933</v>
       </c>
       <c r="H185" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H71</f>
-        <v>91.624000000000024</v>
+        <f>(($B$142*H$174+$A$142)/100)*H70</f>
+        <v>110.17786000000004</v>
       </c>
       <c r="I185" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I71</f>
-        <v>101.79587999999998</v>
+        <f>(($B$142*I$174+$A$142)/100)*I70</f>
+        <v>120.85457999999998</v>
       </c>
       <c r="J185" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J71</f>
-        <v>112.32255999999994</v>
+        <f>(($B$142*J$174+$A$142)/100)*J70</f>
+        <v>135.13807999999992</v>
       </c>
       <c r="K185" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K71</f>
-        <v>133.44388000000004</v>
-      </c>
-      <c r="M185" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K70</f>
+        <v>158.54506000000003</v>
+      </c>
+      <c r="M185" s="54">
         <f t="shared" si="14"/>
-        <v>22.803929628009573</v>
-      </c>
-      <c r="O185" s="49">
-        <v>3.9999999999999999E-16</v>
-      </c>
-      <c r="P185" s="50">
-        <v>2.0199999999999999E-2</v>
+        <v>18.123756746459325</v>
+      </c>
+      <c r="O185" s="4">
+        <f xml:space="preserve"> 0.000000000000001</f>
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="P185" s="40">
+        <v>1.9599999999999999E-2</v>
       </c>
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A186" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B186" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B72</f>
-        <v>45.683700000000002</v>
+        <f>(($B$142*B$174+$A$142)/100)*B71</f>
+        <v>51.62</v>
       </c>
       <c r="C186" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C72</f>
-        <v>45.333539999999985</v>
+        <f>(($B$142*C$174+$A$142)/100)*C71</f>
+        <v>58.503059999999984</v>
       </c>
       <c r="D186" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D72</f>
-        <v>51.671359999999964</v>
+        <f>(($B$142*D$174+$A$142)/100)*D71</f>
+        <v>59.62079999999996</v>
       </c>
       <c r="E186" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E72</f>
-        <v>52.856860000000012</v>
+        <f>(($B$142*E$174+$A$142)/100)*E71</f>
+        <v>71.368940000000009</v>
       </c>
       <c r="F186" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F72</f>
-        <v>63.743579999999987</v>
+        <f>(($B$142*F$174+$A$142)/100)*F71</f>
+        <v>76.635539999999992</v>
       </c>
       <c r="G186" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G72</f>
-        <v>68.532699999999963</v>
+        <f>(($B$142*G$174+$A$142)/100)*G71</f>
+        <v>87.478599999999943</v>
       </c>
       <c r="H186" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H72</f>
-        <v>78.109460000000027</v>
+        <f>(($B$142*H$174+$A$142)/100)*H71</f>
+        <v>91.624000000000024</v>
       </c>
       <c r="I186" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I72</f>
-        <v>82.512959999999993</v>
+        <f>(($B$142*I$174+$A$142)/100)*I71</f>
+        <v>101.79587999999998</v>
       </c>
       <c r="J186" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J72</f>
-        <v>92.578359999999947</v>
+        <f>(($B$142*J$174+$A$142)/100)*J71</f>
+        <v>112.32255999999994</v>
       </c>
       <c r="K186" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K72</f>
-        <v>109.41540000000003</v>
-      </c>
-      <c r="M186" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K71</f>
+        <v>133.44388000000004</v>
+      </c>
+      <c r="M186" s="54">
         <f t="shared" si="14"/>
-        <v>19.286357512430385</v>
-      </c>
-      <c r="O186" s="49">
-        <v>5.9999999999999999E-16</v>
-      </c>
-      <c r="P186" s="50">
-        <v>1.9900000000000001E-2</v>
+        <v>22.803929628009573</v>
+      </c>
+      <c r="O186" s="39">
+        <v>3.9999999999999999E-16</v>
+      </c>
+      <c r="P186" s="40">
+        <v>2.0199999999999999E-2</v>
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A187" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B187" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B73</f>
-        <v>32.778700000000001</v>
+        <f>(($B$142*B$174+$A$142)/100)*B72</f>
+        <v>45.683700000000002</v>
       </c>
       <c r="C187" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C73</f>
-        <v>37.735739999999993</v>
+        <f>(($B$142*C$174+$A$142)/100)*C72</f>
+        <v>45.333539999999985</v>
       </c>
       <c r="D187" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D73</f>
-        <v>37.759839999999976</v>
+        <f>(($B$142*D$174+$A$142)/100)*D72</f>
+        <v>51.671359999999964</v>
       </c>
       <c r="E187" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E73</f>
-        <v>43.357240000000012</v>
+        <f>(($B$142*E$174+$A$142)/100)*E72</f>
+        <v>52.856860000000012</v>
       </c>
       <c r="F187" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F73</f>
-        <v>44.644379999999991</v>
+        <f>(($B$142*F$174+$A$142)/100)*F72</f>
+        <v>63.743579999999987</v>
       </c>
       <c r="G187" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G73</f>
-        <v>54.030899999999967</v>
+        <f>(($B$142*G$174+$A$142)/100)*G72</f>
+        <v>68.532699999999963</v>
       </c>
       <c r="H187" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H73</f>
-        <v>58.181240000000017</v>
+        <f>(($B$142*H$174+$A$142)/100)*H72</f>
+        <v>78.109460000000027</v>
       </c>
       <c r="I187" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I73</f>
-        <v>67.041779999999989</v>
+        <f>(($B$142*I$174+$A$142)/100)*I72</f>
+        <v>82.512959999999993</v>
       </c>
       <c r="J187" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J73</f>
-        <v>71.517879999999963</v>
+        <f>(($B$142*J$174+$A$142)/100)*J72</f>
+        <v>92.578359999999947</v>
       </c>
       <c r="K187" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K73</f>
-        <v>85.816000000000031</v>
-      </c>
-      <c r="M187" s="65">
+        <f>(($B$142*K$174+$A$142)/100)*K72</f>
+        <v>109.41540000000003</v>
+      </c>
+      <c r="M187" s="54">
         <f t="shared" si="14"/>
-        <v>13.333477747336939</v>
-      </c>
-      <c r="O187" s="4">
-        <v>8.9999999999999996E-17</v>
-      </c>
-      <c r="P187" s="50">
-        <v>2.07E-2</v>
+        <v>19.286357512430385</v>
+      </c>
+      <c r="O187" s="39">
+        <v>5.9999999999999999E-16</v>
+      </c>
+      <c r="P187" s="40">
+        <v>1.9900000000000001E-2</v>
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A188" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B188" s="4">
+        <f>(($B$142*B$174+$A$142)/100)*B73</f>
+        <v>32.778700000000001</v>
+      </c>
+      <c r="C188" s="4">
+        <f>(($B$142*C$174+$A$142)/100)*C73</f>
+        <v>37.735739999999993</v>
+      </c>
+      <c r="D188" s="4">
+        <f>(($B$142*D$174+$A$142)/100)*D73</f>
+        <v>37.759839999999976</v>
+      </c>
+      <c r="E188" s="4">
+        <f>(($B$142*E$174+$A$142)/100)*E73</f>
+        <v>43.357240000000012</v>
+      </c>
+      <c r="F188" s="4">
+        <f>(($B$142*F$174+$A$142)/100)*F73</f>
+        <v>44.644379999999991</v>
+      </c>
+      <c r="G188" s="4">
+        <f>(($B$142*G$174+$A$142)/100)*G73</f>
+        <v>54.030899999999967</v>
+      </c>
+      <c r="H188" s="4">
+        <f>(($B$142*H$174+$A$142)/100)*H73</f>
+        <v>58.181240000000017</v>
+      </c>
+      <c r="I188" s="4">
+        <f>(($B$142*I$174+$A$142)/100)*I73</f>
+        <v>67.041779999999989</v>
+      </c>
+      <c r="J188" s="4">
+        <f>(($B$142*J$174+$A$142)/100)*J73</f>
+        <v>71.517879999999963</v>
+      </c>
+      <c r="K188" s="4">
+        <f>(($B$142*K$174+$A$142)/100)*K73</f>
+        <v>85.816000000000031</v>
+      </c>
+      <c r="M188" s="54">
+        <f t="shared" si="14"/>
+        <v>13.333477747336939</v>
+      </c>
+      <c r="O188" s="4">
+        <v>8.9999999999999996E-17</v>
+      </c>
+      <c r="P188" s="40">
+        <v>2.07E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A189" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B188" s="4">
-        <f>(($B$142*B$173+$A$142)/100)*B74</f>
+      <c r="B189" s="4">
+        <f>(($B$142*B$174+$A$142)/100)*B74</f>
         <v>21.938500000000001</v>
       </c>
-      <c r="C188" s="4">
-        <f>(($B$142*C$173+$A$142)/100)*C74</f>
+      <c r="C189" s="4">
+        <f>(($B$142*C$174+$A$142)/100)*C74</f>
         <v>24.566219999999994</v>
       </c>
-      <c r="D188" s="4">
-        <f>(($B$142*D$173+$A$142)/100)*D74</f>
+      <c r="D189" s="4">
+        <f>(($B$142*D$174+$A$142)/100)*D74</f>
         <v>28.568299999999979</v>
       </c>
-      <c r="E188" s="4">
-        <f>(($B$142*E$173+$A$142)/100)*E74</f>
+      <c r="E189" s="4">
+        <f>(($B$142*E$174+$A$142)/100)*E74</f>
         <v>28.742440000000006</v>
       </c>
-      <c r="F188" s="4">
-        <f>(($B$142*F$173+$A$142)/100)*F74</f>
+      <c r="F189" s="4">
+        <f>(($B$142*F$174+$A$142)/100)*F74</f>
         <v>33.184859999999993</v>
       </c>
-      <c r="G188" s="4">
-        <f>(($B$142*G$173+$A$142)/100)*G74</f>
+      <c r="G189" s="4">
+        <f>(($B$142*G$174+$A$142)/100)*G74</f>
         <v>34.383299999999977</v>
       </c>
-      <c r="H188" s="4">
-        <f>(($B$142*H$173+$A$142)/100)*H74</f>
+      <c r="H189" s="4">
+        <f>(($B$142*H$174+$A$142)/100)*H74</f>
         <v>41.917980000000014</v>
       </c>
-      <c r="I188" s="4">
-        <f>(($B$142*I$173+$A$142)/100)*I74</f>
+      <c r="I189" s="4">
+        <f>(($B$142*I$174+$A$142)/100)*I74</f>
         <v>45.740879999999997</v>
       </c>
-      <c r="J188" s="4">
-        <f>(($B$142*J$173+$A$142)/100)*J74</f>
+      <c r="J189" s="4">
+        <f>(($B$142*J$174+$A$142)/100)*J74</f>
         <v>53.748099999999972</v>
       </c>
-      <c r="K188" s="4">
-        <f>(($B$142*K$173+$A$142)/100)*K74</f>
+      <c r="K189" s="4">
+        <f>(($B$142*K$174+$A$142)/100)*K74</f>
         <v>61.143900000000016</v>
       </c>
-      <c r="M188" s="65">
+      <c r="M189" s="54">
         <f t="shared" si="14"/>
         <v>8.591408456529452</v>
       </c>
-      <c r="O188" s="49">
+      <c r="O189" s="39">
         <v>4.0000000000000003E-18</v>
       </c>
-      <c r="P188" s="50">
+      <c r="P189" s="40">
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A189" s="61" t="s">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A190" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B189" s="62">
-        <f>(($B$142*B$173+$A$142)/100)*B75</f>
+      <c r="B190" s="51">
+        <f>(($B$142*B$174+$A$142)/100)*B75</f>
         <v>10.582100000000001</v>
       </c>
-      <c r="C189" s="62">
-        <f>(($B$142*C$173+$A$142)/100)*C75</f>
+      <c r="C190" s="51">
+        <f>(($B$142*C$174+$A$142)/100)*C75</f>
         <v>13.929299999999996</v>
       </c>
-      <c r="D189" s="62">
-        <f>(($B$142*D$173+$A$142)/100)*D75</f>
+      <c r="D190" s="51">
+        <f>(($B$142*D$174+$A$142)/100)*D75</f>
         <v>15.898879999999989</v>
       </c>
-      <c r="E189" s="62">
-        <f>(($B$142*E$173+$A$142)/100)*E75</f>
+      <c r="E190" s="51">
+        <f>(($B$142*E$174+$A$142)/100)*E75</f>
         <v>18.512080000000005</v>
       </c>
-      <c r="F189" s="62">
-        <f>(($B$142*F$173+$A$142)/100)*F75</f>
+      <c r="F190" s="51">
+        <f>(($B$142*F$174+$A$142)/100)*F75</f>
         <v>18.860459999999996</v>
       </c>
-      <c r="G189" s="62">
-        <f>(($B$142*G$173+$A$142)/100)*G75</f>
+      <c r="G190" s="51">
+        <f>(($B$142*G$174+$A$142)/100)*G75</f>
         <v>21.986599999999985</v>
       </c>
-      <c r="H189" s="62">
-        <f>(($B$142*H$173+$A$142)/100)*H75</f>
+      <c r="H190" s="51">
+        <f>(($B$142*H$174+$A$142)/100)*H75</f>
         <v>22.906000000000006</v>
       </c>
-      <c r="I189" s="62">
-        <f>(($B$142*I$173+$A$142)/100)*I75</f>
+      <c r="I190" s="51">
+        <f>(($B$142*I$174+$A$142)/100)*I75</f>
         <v>28.251719999999995</v>
       </c>
-      <c r="J189" s="62">
-        <f>(($B$142*J$173+$A$142)/100)*J75</f>
+      <c r="J190" s="51">
+        <f>(($B$142*J$174+$A$142)/100)*J75</f>
         <v>31.810099999999984</v>
       </c>
-      <c r="K189" s="62">
-        <f>(($B$142*K$173+$A$142)/100)*K75</f>
+      <c r="K190" s="51">
+        <f>(($B$142*K$174+$A$142)/100)*K75</f>
         <v>39.904440000000015</v>
       </c>
-      <c r="M189" s="65">
+      <c r="M190" s="54">
         <f t="shared" si="14"/>
         <v>3.0486932223679761</v>
       </c>
-      <c r="O189" s="49">
+      <c r="O190" s="39">
         <v>9.9999999999999991E-22</v>
       </c>
-      <c r="P189" s="50">
+      <c r="P190" s="40">
         <v>2.5899999999999999E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A190" s="59"/>
-      <c r="B190" s="63">
-        <f>SUM(B174:B187)</f>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A191" s="48"/>
+      <c r="B191" s="52">
+        <f>SUM(B175:B188)</f>
         <v>1699.8466000000001</v>
       </c>
-      <c r="C190" s="63">
-        <f t="shared" ref="C190:K190" si="15">SUM(C174:C187)</f>
+      <c r="C191" s="52">
+        <f t="shared" ref="C191:K191" si="15">SUM(C175:C188)</f>
         <v>1874.6305199999997</v>
       </c>
-      <c r="D190" s="63">
+      <c r="D191" s="52">
         <f t="shared" si="15"/>
         <v>2076.7911999999988</v>
       </c>
-      <c r="E190" s="63">
+      <c r="E191" s="52">
         <f t="shared" si="15"/>
         <v>2315.71506</v>
       </c>
-      <c r="F190" s="63">
+      <c r="F191" s="52">
         <f t="shared" si="15"/>
         <v>2582.4505799999997</v>
       </c>
-      <c r="G190" s="63">
+      <c r="G191" s="52">
         <f t="shared" si="15"/>
         <v>2887.7293999999979</v>
       </c>
-      <c r="H190" s="63">
+      <c r="H191" s="52">
         <f t="shared" si="15"/>
         <v>3203.8622200000013</v>
       </c>
-      <c r="I190" s="63">
+      <c r="I191" s="52">
         <f t="shared" si="15"/>
         <v>3584.8293600000002</v>
       </c>
-      <c r="J190" s="63">
+      <c r="J191" s="52">
         <f t="shared" si="15"/>
         <v>3956.2989199999975</v>
       </c>
-      <c r="K190" s="63">
+      <c r="K191" s="52">
         <f t="shared" si="15"/>
         <v>4374.6851400000014</v>
       </c>
-      <c r="M190" s="56">
-        <f>SUM(M174:M187)</f>
+      <c r="M191" s="45">
+        <f>SUM(M175:M188)</f>
         <v>738.37944363893462</v>
       </c>
     </row>
-    <row r="191" spans="1:16" ht="29" x14ac:dyDescent="0.35">
-      <c r="A191" s="60" t="s">
+    <row r="192" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A192" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B191" s="53">
-        <f>B170+B190</f>
+      <c r="B192" s="42">
+        <f>B171+B191</f>
         <v>3432.9881</v>
       </c>
-      <c r="C191" s="53">
-        <f t="shared" ref="C191:K191" si="16">C170+C190</f>
+      <c r="C192" s="42">
+        <f t="shared" ref="C192:K192" si="16">C171+C191</f>
         <v>3765.4696799999988</v>
       </c>
-      <c r="D191" s="53">
+      <c r="D192" s="42">
         <f t="shared" si="16"/>
         <v>4155.0729199999969</v>
       </c>
-      <c r="E191" s="53">
+      <c r="E192" s="42">
         <f t="shared" si="16"/>
         <v>4620.2254400000002</v>
       </c>
-      <c r="F191" s="53">
+      <c r="F192" s="42">
         <f t="shared" si="16"/>
         <v>5156.0677799999994</v>
       </c>
-      <c r="G191" s="53">
+      <c r="G192" s="42">
         <f t="shared" si="16"/>
         <v>5770.0790999999954</v>
       </c>
-      <c r="H191" s="53">
+      <c r="H192" s="42">
         <f t="shared" si="16"/>
         <v>6399.478280000003</v>
       </c>
-      <c r="I191" s="53">
+      <c r="I192" s="42">
         <f t="shared" si="16"/>
         <v>7166.7438599999996</v>
       </c>
-      <c r="J191" s="53">
+      <c r="J192" s="42">
         <f t="shared" si="16"/>
         <v>7887.1497599999957</v>
       </c>
-      <c r="K191" s="53">
+      <c r="K192" s="42">
         <f t="shared" si="16"/>
         <v>8668.7032400000026</v>
       </c>
-      <c r="M191" s="57">
-        <f>M170+M190</f>
+      <c r="M192" s="46">
+        <f>M171+M191</f>
         <v>1390.6517467890772</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A152:K152"/>
-    <mergeCell ref="A172:K172"/>
+  <mergeCells count="13">
+    <mergeCell ref="A153:K153"/>
+    <mergeCell ref="A173:K173"/>
     <mergeCell ref="A145:A146"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
@@ -18647,6 +18709,7 @@
     <mergeCell ref="A58:P58"/>
     <mergeCell ref="A79:Q79"/>
     <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A150:H150"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Excel description of initial population size calculation
</commit_message>
<xml_diff>
--- a/Config/Population_validation_targets.xlsx
+++ b/Config/Population_validation_targets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2625" windowHeight="2385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="544"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -296,16 +296,16 @@
     <t>Initial population in 1925</t>
   </si>
   <si>
-    <t>Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1925-2002 according to same trend as from 2002-2019. Assume male and female populations by age follow exponential distributions. Highlighted values transferred to Population_data Excel doc.</t>
-  </si>
-  <si>
-    <t>To increase the initial population size, assume an increased slope of the declining provincial share of KZN of the total population, historically</t>
-  </si>
-  <si>
     <t>y=b*exp(mx) --&gt; ln(y)=ln(b)+ln(exp(mx)) --&gt; ln(y)=ln(b)+mx</t>
   </si>
   <si>
     <t>MALES &amp; FEMALES to 69</t>
+  </si>
+  <si>
+    <t>Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1925-2002 according to a slightly steeper trend than that seen from 2002-2019. Assume male and female populations by age follow exponential distributions. Highlighted values transferred to Population_data Excel doc.</t>
+  </si>
+  <si>
+    <t>To increase the initial population size in 1925 and lead to estimates in the 2000s that match observed data, assume an increased slope of the declining provincial share of KZN of the total population, historically compared to that seen in the 2000s</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##0.00;\-##0.00;0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +355,14 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -632,6 +640,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -659,49 +685,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8922,7 +8930,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9531,7 +9538,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14346,8 +14352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G152" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N162" sqref="N162"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14366,16 +14372,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -14397,16 +14403,16 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -15075,16 +15081,16 @@
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -15106,16 +15112,16 @@
       <c r="AA36" s="1"/>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -15137,24 +15143,24 @@
       <c r="AA37" s="1"/>
     </row>
     <row r="38" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="66"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="66"/>
-      <c r="P38" s="67"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="72"/>
+      <c r="N38" s="72"/>
+      <c r="O38" s="72"/>
+      <c r="P38" s="73"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -16073,24 +16079,24 @@
       <c r="A57" s="10"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="59" t="s">
+      <c r="A58" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="60"/>
-      <c r="C58" s="60"/>
-      <c r="D58" s="60"/>
-      <c r="E58" s="60"/>
-      <c r="F58" s="60"/>
-      <c r="G58" s="60"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="60"/>
-      <c r="J58" s="60"/>
-      <c r="K58" s="60"/>
-      <c r="L58" s="60"/>
-      <c r="M58" s="60"/>
-      <c r="N58" s="60"/>
-      <c r="O58" s="60"/>
-      <c r="P58" s="61"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="66"/>
+      <c r="L58" s="66"/>
+      <c r="M58" s="66"/>
+      <c r="N58" s="66"/>
+      <c r="O58" s="66"/>
+      <c r="P58" s="67"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -17071,25 +17077,25 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A79" s="62" t="s">
+      <c r="A79" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="62"/>
-      <c r="C79" s="62"/>
-      <c r="D79" s="62"/>
-      <c r="E79" s="62"/>
-      <c r="F79" s="62"/>
-      <c r="G79" s="62"/>
-      <c r="H79" s="62"/>
-      <c r="I79" s="62"/>
-      <c r="J79" s="62"/>
-      <c r="K79" s="62"/>
-      <c r="L79" s="62"/>
-      <c r="M79" s="62"/>
-      <c r="N79" s="62"/>
-      <c r="O79" s="62"/>
-      <c r="P79" s="62"/>
-      <c r="Q79" s="62"/>
+      <c r="B79" s="68"/>
+      <c r="C79" s="68"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="68"/>
+      <c r="F79" s="68"/>
+      <c r="G79" s="68"/>
+      <c r="H79" s="68"/>
+      <c r="I79" s="68"/>
+      <c r="J79" s="68"/>
+      <c r="K79" s="68"/>
+      <c r="L79" s="68"/>
+      <c r="M79" s="68"/>
+      <c r="N79" s="68"/>
+      <c r="O79" s="68"/>
+      <c r="P79" s="68"/>
+      <c r="Q79" s="68"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
@@ -17320,16 +17326,16 @@
       <c r="A85" s="19"/>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A86" s="63" t="s">
+      <c r="A86" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="B86" s="63"/>
-      <c r="C86" s="63"/>
-      <c r="D86" s="63"/>
-      <c r="E86" s="63"/>
-      <c r="F86" s="63"/>
-      <c r="G86" s="63"/>
-      <c r="H86" s="63"/>
+      <c r="B86" s="69"/>
+      <c r="C86" s="69"/>
+      <c r="D86" s="69"/>
+      <c r="E86" s="69"/>
+      <c r="F86" s="69"/>
+      <c r="G86" s="69"/>
+      <c r="H86" s="69"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -17464,10 +17470,10 @@
       <c r="H90" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="I90" s="72" t="s">
+      <c r="I90" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="J90" s="72"/>
+      <c r="J90" s="63"/>
       <c r="K90" s="21"/>
       <c r="L90" s="24"/>
       <c r="M90" s="25" t="s">
@@ -17486,21 +17492,21 @@
         <v>58</v>
       </c>
       <c r="S90" s="4"/>
-      <c r="T90" s="69" t="s">
+      <c r="T90" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="U90" s="70"/>
-      <c r="V90" s="70"/>
-      <c r="W90" s="70"/>
-      <c r="X90" s="71"/>
+      <c r="U90" s="61"/>
+      <c r="V90" s="61"/>
+      <c r="W90" s="61"/>
+      <c r="X90" s="62"/>
       <c r="Z90" s="4"/>
-      <c r="AA90" s="68" t="s">
+      <c r="AA90" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="AB90" s="68"/>
-      <c r="AC90" s="68"/>
-      <c r="AD90" s="68"/>
-      <c r="AE90" s="68"/>
+      <c r="AB90" s="59"/>
+      <c r="AC90" s="59"/>
+      <c r="AD90" s="59"/>
+      <c r="AE90" s="59"/>
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
@@ -19808,7 +19814,7 @@
       </c>
     </row>
     <row r="145" spans="1:48" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="72" t="s">
+      <c r="A145" s="63" t="s">
         <v>73</v>
       </c>
       <c r="B145" s="38" t="s">
@@ -19880,7 +19886,7 @@
       </c>
     </row>
     <row r="146" spans="1:48" ht="45" x14ac:dyDescent="0.25">
-      <c r="A146" s="72"/>
+      <c r="A146" s="63"/>
       <c r="B146" s="38" t="s">
         <v>75</v>
       </c>
@@ -19981,16 +19987,16 @@
       <c r="AA149" s="1"/>
     </row>
     <row r="150" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A150" s="64" t="s">
+      <c r="A150" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B150" s="64"/>
-      <c r="C150" s="64"/>
-      <c r="D150" s="64"/>
-      <c r="E150" s="64"/>
-      <c r="F150" s="64"/>
-      <c r="G150" s="64"/>
-      <c r="H150" s="64"/>
+      <c r="B150" s="70"/>
+      <c r="C150" s="70"/>
+      <c r="D150" s="70"/>
+      <c r="E150" s="70"/>
+      <c r="F150" s="70"/>
+      <c r="G150" s="70"/>
+      <c r="H150" s="70"/>
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
       <c r="K150" s="1"/>
@@ -20044,7 +20050,7 @@
     </row>
     <row r="152" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A152" s="23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -20073,30 +20079,30 @@
       <c r="Z152" s="1"/>
       <c r="AA152" s="1"/>
     </row>
-    <row r="153" spans="1:48" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="68" t="s">
+    <row r="153" spans="1:48" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B153" s="68"/>
-      <c r="C153" s="68"/>
-      <c r="D153" s="68"/>
-      <c r="E153" s="68"/>
-      <c r="F153" s="68"/>
-      <c r="G153" s="68"/>
-      <c r="H153" s="68"/>
-      <c r="I153" s="68"/>
-      <c r="J153" s="68"/>
-      <c r="K153" s="68"/>
+      <c r="B153" s="59"/>
+      <c r="C153" s="59"/>
+      <c r="D153" s="59"/>
+      <c r="E153" s="59"/>
+      <c r="F153" s="59"/>
+      <c r="G153" s="59"/>
+      <c r="H153" s="59"/>
+      <c r="I153" s="59"/>
+      <c r="J153" s="59"/>
+      <c r="K153" s="59"/>
       <c r="L153" s="41"/>
-      <c r="O153" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="P153" s="82"/>
-      <c r="AC153" s="73" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD153" s="74"/>
-      <c r="AE153" s="75"/>
+      <c r="O153" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="P153" s="64"/>
+      <c r="AC153" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD153" s="75"/>
+      <c r="AE153" s="76"/>
       <c r="AG153" s="33"/>
     </row>
     <row r="154" spans="1:48" x14ac:dyDescent="0.25">
@@ -20142,9 +20148,9 @@
       <c r="P154" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AC154" s="76"/>
-      <c r="AD154" s="77"/>
-      <c r="AE154" s="78"/>
+      <c r="AC154" s="77"/>
+      <c r="AD154" s="78"/>
+      <c r="AE154" s="79"/>
       <c r="AG154" s="33"/>
     </row>
     <row r="155" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20203,9 +20209,9 @@
         <f>INDEX(LINEST(LN(B155:K155),B$154:K$154),1)</f>
         <v>1.5736179276566228E-2</v>
       </c>
-      <c r="AC155" s="79"/>
-      <c r="AD155" s="80"/>
-      <c r="AE155" s="81"/>
+      <c r="AC155" s="80"/>
+      <c r="AD155" s="81"/>
+      <c r="AE155" s="82"/>
       <c r="AG155" s="49"/>
       <c r="AH155" s="49"/>
       <c r="AI155" s="49"/>
@@ -21213,19 +21219,19 @@
       <c r="K172" s="42"/>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A173" s="68" t="s">
+      <c r="A173" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B173" s="68"/>
-      <c r="C173" s="68"/>
-      <c r="D173" s="68"/>
-      <c r="E173" s="68"/>
-      <c r="F173" s="68"/>
-      <c r="G173" s="68"/>
-      <c r="H173" s="68"/>
-      <c r="I173" s="68"/>
-      <c r="J173" s="68"/>
-      <c r="K173" s="68"/>
+      <c r="B173" s="59"/>
+      <c r="C173" s="59"/>
+      <c r="D173" s="59"/>
+      <c r="E173" s="59"/>
+      <c r="F173" s="59"/>
+      <c r="G173" s="59"/>
+      <c r="H173" s="59"/>
+      <c r="I173" s="59"/>
+      <c r="J173" s="59"/>
+      <c r="K173" s="59"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
@@ -22247,7 +22253,7 @@
     </row>
     <row r="192" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="49" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B192" s="42">
         <f>B171+B191</f>
@@ -22296,14 +22302,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="AA90:AE90"/>
-    <mergeCell ref="T90:X90"/>
-    <mergeCell ref="A153:K153"/>
-    <mergeCell ref="A173:K173"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="AC153:AE155"/>
-    <mergeCell ref="O153:P153"/>
     <mergeCell ref="A58:P58"/>
     <mergeCell ref="A79:Q79"/>
     <mergeCell ref="A86:H86"/>
@@ -22313,6 +22311,14 @@
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A38:P38"/>
+    <mergeCell ref="AA90:AE90"/>
+    <mergeCell ref="T90:X90"/>
+    <mergeCell ref="A153:K153"/>
+    <mergeCell ref="A173:K173"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="AC153:AE155"/>
+    <mergeCell ref="O153:P153"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>